<commit_message>
Added explanation on how to use the file
</commit_message>
<xml_diff>
--- a/MLX90640 example data.xlsx
+++ b/MLX90640 example data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="27795" windowHeight="14115" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="27795" windowHeight="14055"/>
   </bookViews>
   <sheets>
     <sheet name="Input data" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10432" uniqueCount="4736">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10446" uniqueCount="4748">
   <si>
     <t>00AE</t>
   </si>
@@ -14271,12 +14271,72 @@
   <si>
     <t>This sheet copntains the calculated To based on the data from sheet 'Input data'</t>
   </si>
+  <si>
+    <t>1. Load the sample EEPROM data into the MCU memory allocated for it.</t>
+  </si>
+  <si>
+    <t>3. Download the calculated parameters and compare to the ones in the sample data file.</t>
+  </si>
+  <si>
+    <t>4. Load the sample frame 0 data into the MCU memory allocated for the frame data and call</t>
+  </si>
+  <si>
+    <t>5. Download the calculated frame temperatures and compare with the ones in the sample data file</t>
+  </si>
+  <si>
+    <t>6. Load the sample frame 1 data into the MCU memory allocated for the frame data and call</t>
+  </si>
+  <si>
+    <t>7. Download the calculated frame temperatures and compare with the ones in the sample data file</t>
+  </si>
+  <si>
+    <t>Verification flow</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. Call the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MLX90640_ExtractParameters(pEEPROM, pParams)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> function</t>
+    </r>
+  </si>
+  <si>
+    <t>tr = MLX90640_GetTa(pFrame, pParams) - 8;</t>
+  </si>
+  <si>
+    <t>MLX90640_CalculateTo(pFrame, pParams, 1.0, tr, pTo);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If all the values you get are the same as the ones in the sample data file, the driver has compiled correctly and all the addressing is intact. </t>
+  </si>
+  <si>
+    <t>All that is left to do is to simply get live data from the sensor and put it in the appropriate memory location.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -14293,6 +14353,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
@@ -14342,7 +14411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -14385,6 +14454,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14686,10 +14761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AFC18"/>
+  <dimension ref="B1:AFC34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22312,8 +22387,82 @@
       <c r="M18" s="18"/>
       <c r="N18" s="18"/>
     </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>4742</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="20" t="s">
+        <v>4736</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="20" t="s">
+        <v>4743</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B23" s="20" t="s">
+        <v>4737</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="20" t="s">
+        <v>4738</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="21" t="s">
+        <v>4744</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="21" t="s">
+        <v>4745</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="20" t="s">
+        <v>4739</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="20" t="s">
+        <v>4740</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="21" t="s">
+        <v>4744</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B30" s="21" t="s">
+        <v>4745</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B31" s="20" t="s">
+        <v>4741</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B32"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>4746</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
+        <v>4747</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -22322,7 +22471,7 @@
   <dimension ref="A2:AI3153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22460,131 +22609,131 @@
         <v>642</v>
       </c>
       <c r="C5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C5)-ROW($C$5))*32+COLUMN(C5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ref="C5:L14" ca="1" si="0">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C5)-ROW($C$5))*32+COLUMN(C5)-COLUMN($C$5),,,"Input data"))</f>
         <v>00AE</v>
       </c>
       <c r="D5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D5)-ROW($C$5))*32+COLUMN(D5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>499A</v>
       </c>
       <c r="E5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E5)-ROW($C$5))*32+COLUMN(E5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0000</v>
       </c>
       <c r="F5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F5)-ROW($C$5))*32+COLUMN(F5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>2061</v>
       </c>
       <c r="G5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G5)-ROW($C$5))*32+COLUMN(G5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0005</v>
       </c>
       <c r="H5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H5)-ROW($C$5))*32+COLUMN(H5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0320</v>
       </c>
       <c r="I5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I5)-ROW($C$5))*32+COLUMN(I5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>03E0</v>
       </c>
       <c r="J5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J5)-ROW($C$5))*32+COLUMN(J5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1710</v>
       </c>
       <c r="K5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K5)-ROW($C$5))*32+COLUMN(K5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>A224</v>
       </c>
       <c r="L5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L5)-ROW($C$5))*32+COLUMN(L5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0185</v>
       </c>
       <c r="M5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M5)-ROW($C$5))*32+COLUMN(M5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ref="M5:V14" ca="1" si="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M5)-ROW($C$5))*32+COLUMN(M5)-COLUMN($C$5),,,"Input data"))</f>
         <v>0499</v>
       </c>
       <c r="N5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N5)-ROW($C$5))*32+COLUMN(N5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0000</v>
       </c>
       <c r="O5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O5)-ROW($C$5))*32+COLUMN(O5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1901</v>
       </c>
       <c r="P5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P5)-ROW($C$5))*32+COLUMN(P5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0000</v>
       </c>
       <c r="Q5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q5)-ROW($C$5))*32+COLUMN(Q5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0000</v>
       </c>
       <c r="R5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R5)-ROW($C$5))*32+COLUMN(R5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>B533</v>
       </c>
       <c r="S5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S5)-ROW($C$5))*32+COLUMN(S5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>4210</v>
       </c>
       <c r="T5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T5)-ROW($C$5))*32+COLUMN(T5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FFC2</v>
       </c>
       <c r="U5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U5)-ROW($C$5))*32+COLUMN(U5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0202</v>
       </c>
       <c r="V5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V5)-ROW($C$5))*32+COLUMN(V5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0202</v>
       </c>
       <c r="W5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W5)-ROW($C$5))*32+COLUMN(W5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ref="W5:AH14" ca="1" si="2">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W5)-ROW($C$5))*32+COLUMN(W5)-COLUMN($C$5),,,"Input data"))</f>
         <v>F202</v>
       </c>
       <c r="X5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X5)-ROW($C$5))*32+COLUMN(X5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F1F2</v>
       </c>
       <c r="Y5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y5)-ROW($C$5))*32+COLUMN(Y5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>D1E1</v>
       </c>
       <c r="Z5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z5)-ROW($C$5))*32+COLUMN(Z5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>AFC0</v>
       </c>
       <c r="AA5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA5)-ROW($C$5))*32+COLUMN(AA5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FF00</v>
       </c>
       <c r="AB5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB5)-ROW($C$5))*32+COLUMN(AB5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F002</v>
       </c>
       <c r="AC5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC5)-ROW($C$5))*32+COLUMN(AC5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F103</v>
       </c>
       <c r="AD5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD5)-ROW($C$5))*32+COLUMN(AD5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>E103</v>
       </c>
       <c r="AE5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE5)-ROW($C$5))*32+COLUMN(AE5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>E1F5</v>
       </c>
       <c r="AF5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF5)-ROW($C$5))*32+COLUMN(AF5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>D1E4</v>
       </c>
       <c r="AG5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG5)-ROW($C$5))*32+COLUMN(AG5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>C1D5</v>
       </c>
       <c r="AH5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH5)-ROW($C$5))*32+COLUMN(AH5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>91C2</v>
       </c>
     </row>
@@ -22594,131 +22743,131 @@
         <v>643</v>
       </c>
       <c r="C6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C6)-ROW($C$5))*32+COLUMN(C6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>8895</v>
       </c>
       <c r="D6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D6)-ROW($C$5))*32+COLUMN(D6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>30D9</v>
       </c>
       <c r="E6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E6)-ROW($C$5))*32+COLUMN(E6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>EDCB</v>
       </c>
       <c r="F6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F6)-ROW($C$5))*32+COLUMN(F6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>110F</v>
       </c>
       <c r="G6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G6)-ROW($C$5))*32+COLUMN(G6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3322</v>
       </c>
       <c r="H6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H6)-ROW($C$5))*32+COLUMN(H6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>2233</v>
       </c>
       <c r="I6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I6)-ROW($C$5))*32+COLUMN(I6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0011</v>
       </c>
       <c r="J6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J6)-ROW($C$5))*32+COLUMN(J6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>CCEE</v>
       </c>
       <c r="K6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K6)-ROW($C$5))*32+COLUMN(K6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FFED</v>
       </c>
       <c r="L6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L6)-ROW($C$5))*32+COLUMN(L6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1100</v>
       </c>
       <c r="M6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M6)-ROW($C$5))*32+COLUMN(M6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>2222</v>
       </c>
       <c r="N6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N6)-ROW($C$5))*32+COLUMN(N6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3333</v>
       </c>
       <c r="O6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O6)-ROW($C$5))*32+COLUMN(O6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>2233</v>
       </c>
       <c r="P6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P6)-ROW($C$5))*32+COLUMN(P6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0022</v>
       </c>
       <c r="Q6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q6)-ROW($C$5))*32+COLUMN(Q6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>DEF0</v>
       </c>
       <c r="R6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R6)-ROW($C$5))*32+COLUMN(R6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>9ACC</v>
       </c>
       <c r="S6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S6)-ROW($C$5))*32+COLUMN(S6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>15CC</v>
       </c>
       <c r="T6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T6)-ROW($C$5))*32+COLUMN(T6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>2FA4</v>
       </c>
       <c r="U6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U6)-ROW($C$5))*32+COLUMN(U6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>2555</v>
       </c>
       <c r="V6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V6)-ROW($C$5))*32+COLUMN(V6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>9C78</v>
       </c>
       <c r="W6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W6)-ROW($C$5))*32+COLUMN(W6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>7666</v>
       </c>
       <c r="X6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X6)-ROW($C$5))*32+COLUMN(X6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>01C8</v>
       </c>
       <c r="Y6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y6)-ROW($C$5))*32+COLUMN(Y6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>3B38</v>
       </c>
       <c r="Z6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z6)-ROW($C$5))*32+COLUMN(Z6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>3534</v>
       </c>
       <c r="AA6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA6)-ROW($C$5))*32+COLUMN(AA6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>2452</v>
       </c>
       <c r="AB6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB6)-ROW($C$5))*32+COLUMN(AB6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0463</v>
       </c>
       <c r="AC6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC6)-ROW($C$5))*32+COLUMN(AC6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>13BB</v>
       </c>
       <c r="AD6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD6)-ROW($C$5))*32+COLUMN(AD6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0623</v>
       </c>
       <c r="AE6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE6)-ROW($C$5))*32+COLUMN(AE6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>EC00</v>
       </c>
       <c r="AF6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF6)-ROW($C$5))*32+COLUMN(AF6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>9797</v>
       </c>
       <c r="AG6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG6)-ROW($C$5))*32+COLUMN(AG6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>9797</v>
       </c>
       <c r="AH6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH6)-ROW($C$5))*32+COLUMN(AH6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>2AFB</v>
       </c>
       <c r="AI6" s="3"/>
@@ -22729,131 +22878,131 @@
         <v>644</v>
       </c>
       <c r="C7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C7)-ROW($C$5))*32+COLUMN(C7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>00AE</v>
       </c>
       <c r="D7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D7)-ROW($C$5))*32+COLUMN(D7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FBE0</v>
       </c>
       <c r="E7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E7)-ROW($C$5))*32+COLUMN(E7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1B70</v>
       </c>
       <c r="F7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F7)-ROW($C$5))*32+COLUMN(F7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>F3BE</v>
       </c>
       <c r="G7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G7)-ROW($C$5))*32+COLUMN(G7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>000E</v>
       </c>
       <c r="H7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H7)-ROW($C$5))*32+COLUMN(H7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>F86E</v>
       </c>
       <c r="I7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I7)-ROW($C$5))*32+COLUMN(I7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1B7E</v>
       </c>
       <c r="J7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J7)-ROW($C$5))*32+COLUMN(J7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>F3CE</v>
       </c>
       <c r="K7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K7)-ROW($C$5))*32+COLUMN(K7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FFCE</v>
       </c>
       <c r="L7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L7)-ROW($C$5))*32+COLUMN(L7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>F41E</v>
       </c>
       <c r="M7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M7)-ROW($C$5))*32+COLUMN(M7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>102E</v>
       </c>
       <c r="N7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N7)-ROW($C$5))*32+COLUMN(N7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>EC0E</v>
       </c>
       <c r="O7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O7)-ROW($C$5))*32+COLUMN(O7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FFDE</v>
       </c>
       <c r="P7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P7)-ROW($C$5))*32+COLUMN(P7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>EC3E</v>
       </c>
       <c r="Q7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q7)-ROW($C$5))*32+COLUMN(Q7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>139E</v>
       </c>
       <c r="R7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R7)-ROW($C$5))*32+COLUMN(R7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>EF9E</v>
       </c>
       <c r="S7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S7)-ROW($C$5))*32+COLUMN(S7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FB9E</v>
       </c>
       <c r="T7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T7)-ROW($C$5))*32+COLUMN(T7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F77E</v>
       </c>
       <c r="U7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U7)-ROW($C$5))*32+COLUMN(U7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>13E0</v>
       </c>
       <c r="V7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V7)-ROW($C$5))*32+COLUMN(V7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>E7EE</v>
       </c>
       <c r="W7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W7)-ROW($C$5))*32+COLUMN(W7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F7AE</v>
       </c>
       <c r="X7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X7)-ROW($C$5))*32+COLUMN(X7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F750</v>
       </c>
       <c r="Y7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y7)-ROW($C$5))*32+COLUMN(Y7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0C30</v>
       </c>
       <c r="Z7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z7)-ROW($C$5))*32+COLUMN(Z7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>EBEE</v>
       </c>
       <c r="AA7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA7)-ROW($C$5))*32+COLUMN(AA7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F730</v>
       </c>
       <c r="AB7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB7)-ROW($C$5))*32+COLUMN(AB7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F010</v>
       </c>
       <c r="AC7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC7)-ROW($C$5))*32+COLUMN(AC7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0B50</v>
       </c>
       <c r="AD7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD7)-ROW($C$5))*32+COLUMN(AD7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>E430</v>
       </c>
       <c r="AE7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE7)-ROW($C$5))*32+COLUMN(AE7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F420</v>
       </c>
       <c r="AF7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF7)-ROW($C$5))*32+COLUMN(AF7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F370</v>
       </c>
       <c r="AG7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG7)-ROW($C$5))*32+COLUMN(AG7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>07C0</v>
       </c>
       <c r="AH7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH7)-ROW($C$5))*32+COLUMN(AH7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>E450</v>
       </c>
     </row>
@@ -22863,131 +23012,131 @@
         <v>645</v>
       </c>
       <c r="C8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C8)-ROW($C$5))*32+COLUMN(C8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0470</v>
       </c>
       <c r="D8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D8)-ROW($C$5))*32+COLUMN(D8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FBCE</v>
       </c>
       <c r="E8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E8)-ROW($C$5))*32+COLUMN(E8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FF5C</v>
       </c>
       <c r="F8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F8)-ROW($C$5))*32+COLUMN(F8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0F90</v>
       </c>
       <c r="G8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G8)-ROW($C$5))*32+COLUMN(G8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>07D0</v>
       </c>
       <c r="H8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H8)-ROW($C$5))*32+COLUMN(H8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FC3E</v>
       </c>
       <c r="I8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I8)-ROW($C$5))*32+COLUMN(I8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FF6C</v>
       </c>
       <c r="J8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J8)-ROW($C$5))*32+COLUMN(J8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0F90</v>
       </c>
       <c r="K8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K8)-ROW($C$5))*32+COLUMN(K8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>03A0</v>
       </c>
       <c r="L8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L8)-ROW($C$5))*32+COLUMN(L8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FC0E</v>
       </c>
       <c r="M8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M8)-ROW($C$5))*32+COLUMN(M8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F40C</v>
       </c>
       <c r="N8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N8)-ROW($C$5))*32+COLUMN(N8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0BF0</v>
       </c>
       <c r="O8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O8)-ROW($C$5))*32+COLUMN(O8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>03A0</v>
       </c>
       <c r="P8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P8)-ROW($C$5))*32+COLUMN(P8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F41E</v>
       </c>
       <c r="Q8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q8)-ROW($C$5))*32+COLUMN(Q8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F78C</v>
       </c>
       <c r="R8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R8)-ROW($C$5))*32+COLUMN(R8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0B70</v>
       </c>
       <c r="S8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S8)-ROW($C$5))*32+COLUMN(S8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FF72</v>
       </c>
       <c r="T8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T8)-ROW($C$5))*32+COLUMN(T8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FF6E</v>
       </c>
       <c r="U8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U8)-ROW($C$5))*32+COLUMN(U8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F7DE</v>
       </c>
       <c r="V8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V8)-ROW($C$5))*32+COLUMN(V8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>07C0</v>
       </c>
       <c r="W8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W8)-ROW($C$5))*32+COLUMN(W8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FFA2</v>
       </c>
       <c r="X8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X8)-ROW($C$5))*32+COLUMN(X8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0330</v>
       </c>
       <c r="Y8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y8)-ROW($C$5))*32+COLUMN(Y8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F42E</v>
       </c>
       <c r="Z8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z8)-ROW($C$5))*32+COLUMN(Z8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0BC0</v>
       </c>
       <c r="AA8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA8)-ROW($C$5))*32+COLUMN(AA8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FF22</v>
       </c>
       <c r="AB8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB8)-ROW($C$5))*32+COLUMN(AB8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FC00</v>
       </c>
       <c r="AC8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC8)-ROW($C$5))*32+COLUMN(AC8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F75E</v>
       </c>
       <c r="AD8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD8)-ROW($C$5))*32+COLUMN(AD8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0410</v>
       </c>
       <c r="AE8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE8)-ROW($C$5))*32+COLUMN(AE8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0022</v>
       </c>
       <c r="AF8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF8)-ROW($C$5))*32+COLUMN(AF8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0350</v>
       </c>
       <c r="AG8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG8)-ROW($C$5))*32+COLUMN(AG8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F3A0</v>
       </c>
       <c r="AH8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH8)-ROW($C$5))*32+COLUMN(AH8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0832</v>
       </c>
     </row>
@@ -22997,131 +23146,131 @@
         <v>646</v>
       </c>
       <c r="C9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C9)-ROW($C$5))*32+COLUMN(C9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>04DE</v>
       </c>
       <c r="D9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D9)-ROW($C$5))*32+COLUMN(D9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FBF0</v>
       </c>
       <c r="E9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E9)-ROW($C$5))*32+COLUMN(E9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1BCE</v>
       </c>
       <c r="F9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F9)-ROW($C$5))*32+COLUMN(F9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>F00E</v>
       </c>
       <c r="G9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G9)-ROW($C$5))*32+COLUMN(G9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FC5E</v>
       </c>
       <c r="H9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H9)-ROW($C$5))*32+COLUMN(H9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FC80</v>
       </c>
       <c r="I9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I9)-ROW($C$5))*32+COLUMN(I9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1BF0</v>
       </c>
       <c r="J9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J9)-ROW($C$5))*32+COLUMN(J9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>F02E</v>
       </c>
       <c r="K9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K9)-ROW($C$5))*32+COLUMN(K9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0002</v>
       </c>
       <c r="L9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L9)-ROW($C$5))*32+COLUMN(L9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>F81E</v>
       </c>
       <c r="M9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M9)-ROW($C$5))*32+COLUMN(M9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>142E</v>
       </c>
       <c r="N9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N9)-ROW($C$5))*32+COLUMN(N9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>EC9E</v>
       </c>
       <c r="O9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O9)-ROW($C$5))*32+COLUMN(O9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>07DE</v>
       </c>
       <c r="P9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P9)-ROW($C$5))*32+COLUMN(P9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F09E</v>
       </c>
       <c r="Q9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q9)-ROW($C$5))*32+COLUMN(Q9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>17CE</v>
       </c>
       <c r="R9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R9)-ROW($C$5))*32+COLUMN(R9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F3AE</v>
       </c>
       <c r="S9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S9)-ROW($C$5))*32+COLUMN(S9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FFC0</v>
       </c>
       <c r="T9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T9)-ROW($C$5))*32+COLUMN(T9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FBB0</v>
       </c>
       <c r="U9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U9)-ROW($C$5))*32+COLUMN(U9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1080</v>
       </c>
       <c r="V9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V9)-ROW($C$5))*32+COLUMN(V9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>EBFE</v>
       </c>
       <c r="W9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W9)-ROW($C$5))*32+COLUMN(W9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FFE0</v>
       </c>
       <c r="X9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X9)-ROW($C$5))*32+COLUMN(X9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FF90</v>
       </c>
       <c r="Y9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y9)-ROW($C$5))*32+COLUMN(Y9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>1460</v>
       </c>
       <c r="Z9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z9)-ROW($C$5))*32+COLUMN(Z9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>E4AE</v>
       </c>
       <c r="AA9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA9)-ROW($C$5))*32+COLUMN(AA9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FBC0</v>
       </c>
       <c r="AB9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB9)-ROW($C$5))*32+COLUMN(AB9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F840</v>
       </c>
       <c r="AC9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC9)-ROW($C$5))*32+COLUMN(AC9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0FE0</v>
       </c>
       <c r="AD9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD9)-ROW($C$5))*32+COLUMN(AD9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>E860</v>
       </c>
       <c r="AE9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE9)-ROW($C$5))*32+COLUMN(AE9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F8C0</v>
       </c>
       <c r="AF9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF9)-ROW($C$5))*32+COLUMN(AF9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F400</v>
       </c>
       <c r="AG9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG9)-ROW($C$5))*32+COLUMN(AG9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0842</v>
       </c>
       <c r="AH9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH9)-ROW($C$5))*32+COLUMN(AH9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>E4B0</v>
       </c>
     </row>
@@ -23131,131 +23280,131 @@
         <v>647</v>
       </c>
       <c r="C10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C10)-ROW($C$5))*32+COLUMN(C10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0890</v>
       </c>
       <c r="D10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D10)-ROW($C$5))*32+COLUMN(D10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>03BE</v>
       </c>
       <c r="E10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E10)-ROW($C$5))*32+COLUMN(E10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FF9C</v>
       </c>
       <c r="F10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F10)-ROW($C$5))*32+COLUMN(F10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0FD0</v>
       </c>
       <c r="G10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G10)-ROW($C$5))*32+COLUMN(G10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0020</v>
       </c>
       <c r="H10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H10)-ROW($C$5))*32+COLUMN(H10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0450</v>
       </c>
       <c r="I10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I10)-ROW($C$5))*32+COLUMN(I10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FFCC</v>
       </c>
       <c r="J10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J10)-ROW($C$5))*32+COLUMN(J10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0FE0</v>
       </c>
       <c r="K10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K10)-ROW($C$5))*32+COLUMN(K10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>07D0</v>
       </c>
       <c r="L10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L10)-ROW($C$5))*32+COLUMN(L10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>03FE</v>
       </c>
       <c r="M10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M10)-ROW($C$5))*32+COLUMN(M10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FBEE</v>
       </c>
       <c r="N10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N10)-ROW($C$5))*32+COLUMN(N10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0C60</v>
       </c>
       <c r="O10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O10)-ROW($C$5))*32+COLUMN(O10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0B80</v>
       </c>
       <c r="P10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P10)-ROW($C$5))*32+COLUMN(P10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F86E</v>
       </c>
       <c r="Q10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q10)-ROW($C$5))*32+COLUMN(Q10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FB8E</v>
       </c>
       <c r="R10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R10)-ROW($C$5))*32+COLUMN(R10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1370</v>
       </c>
       <c r="S10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S10)-ROW($C$5))*32+COLUMN(S10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0782</v>
       </c>
       <c r="T10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T10)-ROW($C$5))*32+COLUMN(T10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>038E</v>
       </c>
       <c r="U10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U10)-ROW($C$5))*32+COLUMN(U10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F85E</v>
       </c>
       <c r="V10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V10)-ROW($C$5))*32+COLUMN(V10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0FC2</v>
       </c>
       <c r="W10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W10)-ROW($C$5))*32+COLUMN(W10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>07C2</v>
       </c>
       <c r="X10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X10)-ROW($C$5))*32+COLUMN(X10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>037E</v>
       </c>
       <c r="Y10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y10)-ROW($C$5))*32+COLUMN(Y10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F84E</v>
       </c>
       <c r="Z10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z10)-ROW($C$5))*32+COLUMN(Z10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0880</v>
       </c>
       <c r="AA10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA10)-ROW($C$5))*32+COLUMN(AA10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0392</v>
       </c>
       <c r="AB10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB10)-ROW($C$5))*32+COLUMN(AB10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0420</v>
       </c>
       <c r="AC10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC10)-ROW($C$5))*32+COLUMN(AC10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F7CE</v>
       </c>
       <c r="AD10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD10)-ROW($C$5))*32+COLUMN(AD10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0C42</v>
       </c>
       <c r="AE10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE10)-ROW($C$5))*32+COLUMN(AE10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FCB2</v>
       </c>
       <c r="AF10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF10)-ROW($C$5))*32+COLUMN(AF10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FFE0</v>
       </c>
       <c r="AG10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG10)-ROW($C$5))*32+COLUMN(AG10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F020</v>
       </c>
       <c r="AH10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH10)-ROW($C$5))*32+COLUMN(AH10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0490</v>
       </c>
     </row>
@@ -23265,131 +23414,131 @@
         <v>648</v>
       </c>
       <c r="C11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C11)-ROW($C$5))*32+COLUMN(C11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>107E</v>
       </c>
       <c r="D11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D11)-ROW($C$5))*32+COLUMN(D11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>03D0</v>
       </c>
       <c r="E11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E11)-ROW($C$5))*32+COLUMN(E11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1F90</v>
       </c>
       <c r="F11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F11)-ROW($C$5))*32+COLUMN(F11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FBCE</v>
       </c>
       <c r="G11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G11)-ROW($C$5))*32+COLUMN(G11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>089E</v>
       </c>
       <c r="H11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H11)-ROW($C$5))*32+COLUMN(H11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0080</v>
       </c>
       <c r="I11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I11)-ROW($C$5))*32+COLUMN(I11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1820</v>
       </c>
       <c r="J11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J11)-ROW($C$5))*32+COLUMN(J11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>F40E</v>
       </c>
       <c r="K11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K11)-ROW($C$5))*32+COLUMN(K11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0800</v>
       </c>
       <c r="L11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L11)-ROW($C$5))*32+COLUMN(L11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FC30</v>
       </c>
       <c r="M11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M11)-ROW($C$5))*32+COLUMN(M11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>141E</v>
       </c>
       <c r="N11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N11)-ROW($C$5))*32+COLUMN(N11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F06E</v>
       </c>
       <c r="O11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O11)-ROW($C$5))*32+COLUMN(O11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0400</v>
       </c>
       <c r="P11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P11)-ROW($C$5))*32+COLUMN(P11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FFA0</v>
       </c>
       <c r="Q11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q11)-ROW($C$5))*32+COLUMN(Q11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>17CE</v>
       </c>
       <c r="R11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R11)-ROW($C$5))*32+COLUMN(R11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F7B0</v>
       </c>
       <c r="S11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S11)-ROW($C$5))*32+COLUMN(S11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>07D0</v>
       </c>
       <c r="T11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T11)-ROW($C$5))*32+COLUMN(T11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FFB0</v>
       </c>
       <c r="U11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U11)-ROW($C$5))*32+COLUMN(U11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1830</v>
       </c>
       <c r="V11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V11)-ROW($C$5))*32+COLUMN(V11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F3FE</v>
       </c>
       <c r="W11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W11)-ROW($C$5))*32+COLUMN(W11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0002</v>
       </c>
       <c r="X11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X11)-ROW($C$5))*32+COLUMN(X11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FFE0</v>
       </c>
       <c r="Y11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y11)-ROW($C$5))*32+COLUMN(Y11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>14D0</v>
       </c>
       <c r="Z11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z11)-ROW($C$5))*32+COLUMN(Z11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>ECB0</v>
       </c>
       <c r="AA11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA11)-ROW($C$5))*32+COLUMN(AA11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FBE2</v>
       </c>
       <c r="AB11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB11)-ROW($C$5))*32+COLUMN(AB11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FCB0</v>
       </c>
       <c r="AC11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC11)-ROW($C$5))*32+COLUMN(AC11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>13B0</v>
       </c>
       <c r="AD11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD11)-ROW($C$5))*32+COLUMN(AD11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>ECA0</v>
       </c>
       <c r="AE11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE11)-ROW($C$5))*32+COLUMN(AE11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F8DE</v>
       </c>
       <c r="AF11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF11)-ROW($C$5))*32+COLUMN(AF11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F432</v>
       </c>
       <c r="AG11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG11)-ROW($C$5))*32+COLUMN(AG11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0832</v>
       </c>
       <c r="AH11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH11)-ROW($C$5))*32+COLUMN(AH11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>E8D0</v>
       </c>
     </row>
@@ -23399,131 +23548,131 @@
         <v>649</v>
       </c>
       <c r="C12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C12)-ROW($C$5))*32+COLUMN(C12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1420</v>
       </c>
       <c r="D12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D12)-ROW($C$5))*32+COLUMN(D12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FF8E</v>
       </c>
       <c r="E12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E12)-ROW($C$5))*32+COLUMN(E12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FF6E</v>
       </c>
       <c r="F12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F12)-ROW($C$5))*32+COLUMN(F12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1380</v>
       </c>
       <c r="G12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G12)-ROW($C$5))*32+COLUMN(G12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0840</v>
       </c>
       <c r="H12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H12)-ROW($C$5))*32+COLUMN(H12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>005E</v>
       </c>
       <c r="I12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I12)-ROW($C$5))*32+COLUMN(I12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FBEC</v>
       </c>
       <c r="J12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J12)-ROW($C$5))*32+COLUMN(J12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0FB0</v>
       </c>
       <c r="K12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K12)-ROW($C$5))*32+COLUMN(K12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0BB2</v>
       </c>
       <c r="L12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L12)-ROW($C$5))*32+COLUMN(L12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FFFE</v>
       </c>
       <c r="M12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M12)-ROW($C$5))*32+COLUMN(M12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FBDE</v>
       </c>
       <c r="N12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N12)-ROW($C$5))*32+COLUMN(N12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0820</v>
       </c>
       <c r="O12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O12)-ROW($C$5))*32+COLUMN(O12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0BC0</v>
       </c>
       <c r="P12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P12)-ROW($C$5))*32+COLUMN(P12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0360</v>
       </c>
       <c r="Q12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q12)-ROW($C$5))*32+COLUMN(Q12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FB8C</v>
       </c>
       <c r="R12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R12)-ROW($C$5))*32+COLUMN(R12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0F70</v>
       </c>
       <c r="S12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S12)-ROW($C$5))*32+COLUMN(S12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0794</v>
       </c>
       <c r="T12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T12)-ROW($C$5))*32+COLUMN(T12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>036E</v>
       </c>
       <c r="U12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U12)-ROW($C$5))*32+COLUMN(U12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FBFE</v>
       </c>
       <c r="V12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V12)-ROW($C$5))*32+COLUMN(V12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0FA0</v>
       </c>
       <c r="W12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W12)-ROW($C$5))*32+COLUMN(W12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0BC4</v>
       </c>
       <c r="X12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X12)-ROW($C$5))*32+COLUMN(X12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0390</v>
       </c>
       <c r="Y12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y12)-ROW($C$5))*32+COLUMN(Y12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F89E</v>
       </c>
       <c r="Z12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z12)-ROW($C$5))*32+COLUMN(Z12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0C72</v>
       </c>
       <c r="AA12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA12)-ROW($C$5))*32+COLUMN(AA12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FFB2</v>
       </c>
       <c r="AB12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB12)-ROW($C$5))*32+COLUMN(AB12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FC70</v>
       </c>
       <c r="AC12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC12)-ROW($C$5))*32+COLUMN(AC12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FB7E</v>
       </c>
       <c r="AD12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD12)-ROW($C$5))*32+COLUMN(AD12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0470</v>
       </c>
       <c r="AE12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE12)-ROW($C$5))*32+COLUMN(AE12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FCB0</v>
       </c>
       <c r="AF12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF12)-ROW($C$5))*32+COLUMN(AF12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FFF0</v>
       </c>
       <c r="AG12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG12)-ROW($C$5))*32+COLUMN(AG12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F3F0</v>
       </c>
       <c r="AH12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH12)-ROW($C$5))*32+COLUMN(AH12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>04A0</v>
       </c>
     </row>
@@ -23533,131 +23682,131 @@
         <v>650</v>
       </c>
       <c r="C13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C13)-ROW($C$5))*32+COLUMN(C13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>049E</v>
       </c>
       <c r="D13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D13)-ROW($C$5))*32+COLUMN(D13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>03B0</v>
       </c>
       <c r="E13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E13)-ROW($C$5))*32+COLUMN(E13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1F90</v>
       </c>
       <c r="F13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F13)-ROW($C$5))*32+COLUMN(F13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>F7D0</v>
       </c>
       <c r="G13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G13)-ROW($C$5))*32+COLUMN(G13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>042E</v>
       </c>
       <c r="H13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H13)-ROW($C$5))*32+COLUMN(H13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0070</v>
       </c>
       <c r="I13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I13)-ROW($C$5))*32+COLUMN(I13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1F70</v>
       </c>
       <c r="J13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J13)-ROW($C$5))*32+COLUMN(J13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FBBE</v>
       </c>
       <c r="K13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K13)-ROW($C$5))*32+COLUMN(K13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0F00</v>
       </c>
       <c r="L13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L13)-ROW($C$5))*32+COLUMN(L13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>03B0</v>
       </c>
       <c r="M13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M13)-ROW($C$5))*32+COLUMN(M13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>142E</v>
       </c>
       <c r="N13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N13)-ROW($C$5))*32+COLUMN(N13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F01E</v>
       </c>
       <c r="O13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O13)-ROW($C$5))*32+COLUMN(O13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>07B0</v>
       </c>
       <c r="P13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P13)-ROW($C$5))*32+COLUMN(P13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FFB0</v>
       </c>
       <c r="Q13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q13)-ROW($C$5))*32+COLUMN(Q13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1B60</v>
       </c>
       <c r="R13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R13)-ROW($C$5))*32+COLUMN(R13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F37E</v>
       </c>
       <c r="S13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S13)-ROW($C$5))*32+COLUMN(S13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FBD0</v>
       </c>
       <c r="T13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T13)-ROW($C$5))*32+COLUMN(T13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FF90</v>
       </c>
       <c r="U13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U13)-ROW($C$5))*32+COLUMN(U13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1410</v>
       </c>
       <c r="V13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V13)-ROW($C$5))*32+COLUMN(V13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F3C0</v>
       </c>
       <c r="W13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W13)-ROW($C$5))*32+COLUMN(W13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FC00</v>
       </c>
       <c r="X13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X13)-ROW($C$5))*32+COLUMN(X13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0370</v>
       </c>
       <c r="Y13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y13)-ROW($C$5))*32+COLUMN(Y13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>1482</v>
       </c>
       <c r="Z13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z13)-ROW($C$5))*32+COLUMN(Z13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F030</v>
       </c>
       <c r="AA13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA13)-ROW($C$5))*32+COLUMN(AA13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F800</v>
       </c>
       <c r="AB13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB13)-ROW($C$5))*32+COLUMN(AB13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FC50</v>
       </c>
       <c r="AC13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC13)-ROW($C$5))*32+COLUMN(AC13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>13C2</v>
       </c>
       <c r="AD13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD13)-ROW($C$5))*32+COLUMN(AD13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F050</v>
       </c>
       <c r="AE13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE13)-ROW($C$5))*32+COLUMN(AE13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0070</v>
       </c>
       <c r="AF13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF13)-ROW($C$5))*32+COLUMN(AF13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F812</v>
       </c>
       <c r="AG13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG13)-ROW($C$5))*32+COLUMN(AG13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0C02</v>
       </c>
       <c r="AH13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH13)-ROW($C$5))*32+COLUMN(AH13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>EC80</v>
       </c>
     </row>
@@ -23667,131 +23816,131 @@
         <v>651</v>
       </c>
       <c r="C14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C14)-ROW($C$5))*32+COLUMN(C14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>00D0</v>
       </c>
       <c r="D14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D14)-ROW($C$5))*32+COLUMN(D14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FBFE</v>
       </c>
       <c r="E14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E14)-ROW($C$5))*32+COLUMN(E14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FBCC</v>
       </c>
       <c r="F14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F14)-ROW($C$5))*32+COLUMN(F14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0810</v>
       </c>
       <c r="G14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G14)-ROW($C$5))*32+COLUMN(G14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FC60</v>
       </c>
       <c r="H14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H14)-ROW($C$5))*32+COLUMN(H14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FCB0</v>
       </c>
       <c r="I14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I14)-ROW($C$5))*32+COLUMN(I14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FBCE</v>
       </c>
       <c r="J14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J14)-ROW($C$5))*32+COLUMN(J14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0FE0</v>
       </c>
       <c r="K14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K14)-ROW($C$5))*32+COLUMN(K14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0B40</v>
       </c>
       <c r="L14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L14)-ROW($C$5))*32+COLUMN(L14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FFFE</v>
       </c>
       <c r="M14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M14)-ROW($C$5))*32+COLUMN(M14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F05C</v>
       </c>
       <c r="N14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N14)-ROW($C$5))*32+COLUMN(N14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0840</v>
       </c>
       <c r="O14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O14)-ROW($C$5))*32+COLUMN(O14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>07D0</v>
       </c>
       <c r="P14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P14)-ROW($C$5))*32+COLUMN(P14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FFD0</v>
       </c>
       <c r="Q14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q14)-ROW($C$5))*32+COLUMN(Q14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F79E</v>
       </c>
       <c r="R14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R14)-ROW($C$5))*32+COLUMN(R14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0FB0</v>
       </c>
       <c r="S14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S14)-ROW($C$5))*32+COLUMN(S14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F802</v>
       </c>
       <c r="T14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T14)-ROW($C$5))*32+COLUMN(T14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FFD0</v>
       </c>
       <c r="U14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U14)-ROW($C$5))*32+COLUMN(U14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F44E</v>
       </c>
       <c r="V14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V14)-ROW($C$5))*32+COLUMN(V14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0BF0</v>
       </c>
       <c r="W14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W14)-ROW($C$5))*32+COLUMN(W14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FC32</v>
       </c>
       <c r="X14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X14)-ROW($C$5))*32+COLUMN(X14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>07A0</v>
       </c>
       <c r="Y14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y14)-ROW($C$5))*32+COLUMN(Y14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F4BE</v>
       </c>
       <c r="Z14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z14)-ROW($C$5))*32+COLUMN(Z14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0C60</v>
       </c>
       <c r="AA14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA14)-ROW($C$5))*32+COLUMN(AA14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F822</v>
       </c>
       <c r="AB14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB14)-ROW($C$5))*32+COLUMN(AB14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0080</v>
       </c>
       <c r="AC14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC14)-ROW($C$5))*32+COLUMN(AC14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F01E</v>
       </c>
       <c r="AD14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD14)-ROW($C$5))*32+COLUMN(AD14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0892</v>
       </c>
       <c r="AE14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE14)-ROW($C$5))*32+COLUMN(AE14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>00B4</v>
       </c>
       <c r="AF14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF14)-ROW($C$5))*32+COLUMN(AF14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F850</v>
       </c>
       <c r="AG14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG14)-ROW($C$5))*32+COLUMN(AG14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F040</v>
       </c>
       <c r="AH14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH14)-ROW($C$5))*32+COLUMN(AH14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>04B2</v>
       </c>
     </row>
@@ -23801,131 +23950,131 @@
         <v>652</v>
       </c>
       <c r="C15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C15)-ROW($C$5))*32+COLUMN(C15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ref="C15:L24" ca="1" si="3">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C15)-ROW($C$5))*32+COLUMN(C15)-COLUMN($C$5),,,"Input data"))</f>
         <v>085E</v>
       </c>
       <c r="D15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D15)-ROW($C$5))*32+COLUMN(D15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0782</v>
       </c>
       <c r="E15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E15)-ROW($C$5))*32+COLUMN(E15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1F70</v>
       </c>
       <c r="F15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F15)-ROW($C$5))*32+COLUMN(F15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FBEE</v>
       </c>
       <c r="G15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G15)-ROW($C$5))*32+COLUMN(G15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>001E</v>
       </c>
       <c r="H15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H15)-ROW($C$5))*32+COLUMN(H15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0420</v>
       </c>
       <c r="I15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I15)-ROW($C$5))*32+COLUMN(I15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1F80</v>
       </c>
       <c r="J15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J15)-ROW($C$5))*32+COLUMN(J15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FBB0</v>
       </c>
       <c r="K15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K15)-ROW($C$5))*32+COLUMN(K15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>03B0</v>
       </c>
       <c r="L15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L15)-ROW($C$5))*32+COLUMN(L15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0390</v>
       </c>
       <c r="M15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M15)-ROW($C$5))*32+COLUMN(M15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ref="M15:V24" ca="1" si="4">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M15)-ROW($C$5))*32+COLUMN(M15)-COLUMN($C$5),,,"Input data"))</f>
         <v>17F0</v>
       </c>
       <c r="N15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N15)-ROW($C$5))*32+COLUMN(N15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F04E</v>
       </c>
       <c r="O15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O15)-ROW($C$5))*32+COLUMN(O15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0770</v>
       </c>
       <c r="P15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P15)-ROW($C$5))*32+COLUMN(P15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FFE0</v>
       </c>
       <c r="Q15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q15)-ROW($C$5))*32+COLUMN(Q15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1B40</v>
       </c>
       <c r="R15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R15)-ROW($C$5))*32+COLUMN(R15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F76E</v>
       </c>
       <c r="S15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S15)-ROW($C$5))*32+COLUMN(S15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FFC0</v>
       </c>
       <c r="T15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T15)-ROW($C$5))*32+COLUMN(T15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FFB0</v>
       </c>
       <c r="U15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U15)-ROW($C$5))*32+COLUMN(U15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>17E0</v>
       </c>
       <c r="V15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V15)-ROW($C$5))*32+COLUMN(V15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>EC1E</v>
       </c>
       <c r="W15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W15)-ROW($C$5))*32+COLUMN(W15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ref="W15:AH24" ca="1" si="5">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W15)-ROW($C$5))*32+COLUMN(W15)-COLUMN($C$5),,,"Input data"))</f>
         <v>03A0</v>
       </c>
       <c r="X15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X15)-ROW($C$5))*32+COLUMN(X15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>03A0</v>
       </c>
       <c r="Y15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y15)-ROW($C$5))*32+COLUMN(Y15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>10C0</v>
       </c>
       <c r="Z15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z15)-ROW($C$5))*32+COLUMN(Z15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>EC60</v>
       </c>
       <c r="AA15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA15)-ROW($C$5))*32+COLUMN(AA15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FBC2</v>
       </c>
       <c r="AB15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB15)-ROW($C$5))*32+COLUMN(AB15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FC80</v>
       </c>
       <c r="AC15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC15)-ROW($C$5))*32+COLUMN(AC15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0C00</v>
       </c>
       <c r="AD15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD15)-ROW($C$5))*32+COLUMN(AD15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>EC60</v>
       </c>
       <c r="AE15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE15)-ROW($C$5))*32+COLUMN(AE15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0050</v>
       </c>
       <c r="AF15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF15)-ROW($C$5))*32+COLUMN(AF15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F800</v>
       </c>
       <c r="AG15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG15)-ROW($C$5))*32+COLUMN(AG15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0802</v>
       </c>
       <c r="AH15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH15)-ROW($C$5))*32+COLUMN(AH15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>EC90</v>
       </c>
     </row>
@@ -23935,131 +24084,131 @@
         <v>653</v>
       </c>
       <c r="C16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C16)-ROW($C$5))*32+COLUMN(C16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0080</v>
       </c>
       <c r="D16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D16)-ROW($C$5))*32+COLUMN(D16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F7B0</v>
       </c>
       <c r="E16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E16)-ROW($C$5))*32+COLUMN(E16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F7AE</v>
       </c>
       <c r="F16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F16)-ROW($C$5))*32+COLUMN(F16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0410</v>
       </c>
       <c r="G16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G16)-ROW($C$5))*32+COLUMN(G16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FC32</v>
       </c>
       <c r="H16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H16)-ROW($C$5))*32+COLUMN(H16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FC50</v>
       </c>
       <c r="I16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I16)-ROW($C$5))*32+COLUMN(I16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F7BE</v>
       </c>
       <c r="J16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J16)-ROW($C$5))*32+COLUMN(J16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>07F0</v>
       </c>
       <c r="K16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K16)-ROW($C$5))*32+COLUMN(K16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FFD2</v>
       </c>
       <c r="L16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L16)-ROW($C$5))*32+COLUMN(L16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FBC0</v>
       </c>
       <c r="M16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M16)-ROW($C$5))*32+COLUMN(M16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F02E</v>
       </c>
       <c r="N16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N16)-ROW($C$5))*32+COLUMN(N16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0460</v>
       </c>
       <c r="O16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O16)-ROW($C$5))*32+COLUMN(O16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0382</v>
       </c>
       <c r="P16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P16)-ROW($C$5))*32+COLUMN(P16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F410</v>
       </c>
       <c r="Q16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q16)-ROW($C$5))*32+COLUMN(Q16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F36E</v>
       </c>
       <c r="R16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R16)-ROW($C$5))*32+COLUMN(R16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0BA0</v>
       </c>
       <c r="S16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S16)-ROW($C$5))*32+COLUMN(S16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FBF2</v>
       </c>
       <c r="T16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T16)-ROW($C$5))*32+COLUMN(T16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FBC0</v>
       </c>
       <c r="U16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U16)-ROW($C$5))*32+COLUMN(U16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F01C</v>
       </c>
       <c r="V16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V16)-ROW($C$5))*32+COLUMN(V16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0440</v>
       </c>
       <c r="W16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W16)-ROW($C$5))*32+COLUMN(W16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FFE2</v>
       </c>
       <c r="X16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X16)-ROW($C$5))*32+COLUMN(X16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FBE0</v>
       </c>
       <c r="Y16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y16)-ROW($C$5))*32+COLUMN(Y16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F0EE</v>
       </c>
       <c r="Z16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z16)-ROW($C$5))*32+COLUMN(Z16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>08A2</v>
       </c>
       <c r="AA16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA16)-ROW($C$5))*32+COLUMN(AA16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F804</v>
       </c>
       <c r="AB16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB16)-ROW($C$5))*32+COLUMN(AB16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FCB0</v>
       </c>
       <c r="AC16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC16)-ROW($C$5))*32+COLUMN(AC16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>EC3E</v>
       </c>
       <c r="AD16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD16)-ROW($C$5))*32+COLUMN(AD16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>04A2</v>
       </c>
       <c r="AE16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE16)-ROW($C$5))*32+COLUMN(AE16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0082</v>
       </c>
       <c r="AF16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF16)-ROW($C$5))*32+COLUMN(AF16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F830</v>
       </c>
       <c r="AG16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG16)-ROW($C$5))*32+COLUMN(AG16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>E830</v>
       </c>
       <c r="AH16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH16)-ROW($C$5))*32+COLUMN(AH16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>04B2</v>
       </c>
     </row>
@@ -24069,131 +24218,131 @@
         <v>654</v>
       </c>
       <c r="C17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C17)-ROW($C$5))*32+COLUMN(C17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>13F0</v>
       </c>
       <c r="D17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D17)-ROW($C$5))*32+COLUMN(D17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0380</v>
       </c>
       <c r="E17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E17)-ROW($C$5))*32+COLUMN(E17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1F40</v>
       </c>
       <c r="F17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F17)-ROW($C$5))*32+COLUMN(F17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FBB0</v>
       </c>
       <c r="G17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G17)-ROW($C$5))*32+COLUMN(G17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0F90</v>
       </c>
       <c r="H17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H17)-ROW($C$5))*32+COLUMN(H17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0420</v>
       </c>
       <c r="I17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I17)-ROW($C$5))*32+COLUMN(I17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>17A0</v>
       </c>
       <c r="J17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J17)-ROW($C$5))*32+COLUMN(J17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F7AE</v>
       </c>
       <c r="K17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K17)-ROW($C$5))*32+COLUMN(K17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0F40</v>
       </c>
       <c r="L17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L17)-ROW($C$5))*32+COLUMN(L17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FFE2</v>
       </c>
       <c r="M17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M17)-ROW($C$5))*32+COLUMN(M17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>13AE</v>
       </c>
       <c r="N17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N17)-ROW($C$5))*32+COLUMN(N17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F03E</v>
       </c>
       <c r="O17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O17)-ROW($C$5))*32+COLUMN(O17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0F12</v>
       </c>
       <c r="P17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P17)-ROW($C$5))*32+COLUMN(P17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FF60</v>
       </c>
       <c r="Q17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q17)-ROW($C$5))*32+COLUMN(Q17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0F50</v>
       </c>
       <c r="R17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R17)-ROW($C$5))*32+COLUMN(R17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F340</v>
       </c>
       <c r="S17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S17)-ROW($C$5))*32+COLUMN(S17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0362</v>
       </c>
       <c r="T17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T17)-ROW($C$5))*32+COLUMN(T17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FF30</v>
       </c>
       <c r="U17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U17)-ROW($C$5))*32+COLUMN(U17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1760</v>
       </c>
       <c r="V17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V17)-ROW($C$5))*32+COLUMN(V17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>EFD0</v>
       </c>
       <c r="W17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W17)-ROW($C$5))*32+COLUMN(W17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0762</v>
       </c>
       <c r="X17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X17)-ROW($C$5))*32+COLUMN(X17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0360</v>
       </c>
       <c r="Y17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y17)-ROW($C$5))*32+COLUMN(Y17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>1072</v>
       </c>
       <c r="Z17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z17)-ROW($C$5))*32+COLUMN(Z17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>EC50</v>
       </c>
       <c r="AA17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA17)-ROW($C$5))*32+COLUMN(AA17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F7B2</v>
       </c>
       <c r="AB17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB17)-ROW($C$5))*32+COLUMN(AB17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F852</v>
       </c>
       <c r="AC17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC17)-ROW($C$5))*32+COLUMN(AC17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>07B0</v>
       </c>
       <c r="AD17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD17)-ROW($C$5))*32+COLUMN(AD17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>E480</v>
       </c>
       <c r="AE17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE17)-ROW($C$5))*32+COLUMN(AE17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F820</v>
       </c>
       <c r="AF17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF17)-ROW($C$5))*32+COLUMN(AF17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F7C2</v>
       </c>
       <c r="AG17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG17)-ROW($C$5))*32+COLUMN(AG17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>03C2</v>
       </c>
       <c r="AH17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH17)-ROW($C$5))*32+COLUMN(AH17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>E490</v>
       </c>
     </row>
@@ -24203,131 +24352,131 @@
         <v>655</v>
       </c>
       <c r="C18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C18)-ROW($C$5))*32+COLUMN(C18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1422</v>
       </c>
       <c r="D18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D18)-ROW($C$5))*32+COLUMN(D18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>03AE</v>
       </c>
       <c r="E18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E18)-ROW($C$5))*32+COLUMN(E18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>036E</v>
       </c>
       <c r="F18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F18)-ROW($C$5))*32+COLUMN(F18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>13C2</v>
       </c>
       <c r="G18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G18)-ROW($C$5))*32+COLUMN(G18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>13B2</v>
       </c>
       <c r="H18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H18)-ROW($C$5))*32+COLUMN(H18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0440</v>
       </c>
       <c r="I18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I18)-ROW($C$5))*32+COLUMN(I18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FFCE</v>
       </c>
       <c r="J18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J18)-ROW($C$5))*32+COLUMN(J18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>13D2</v>
       </c>
       <c r="K18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K18)-ROW($C$5))*32+COLUMN(K18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1362</v>
       </c>
       <c r="L18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L18)-ROW($C$5))*32+COLUMN(L18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0002</v>
       </c>
       <c r="M18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M18)-ROW($C$5))*32+COLUMN(M18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FBDE</v>
       </c>
       <c r="N18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N18)-ROW($C$5))*32+COLUMN(N18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0C40</v>
       </c>
       <c r="O18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O18)-ROW($C$5))*32+COLUMN(O18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1732</v>
       </c>
       <c r="P18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P18)-ROW($C$5))*32+COLUMN(P18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0390</v>
       </c>
       <c r="Q18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q18)-ROW($C$5))*32+COLUMN(Q18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FF8E</v>
       </c>
       <c r="R18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R18)-ROW($C$5))*32+COLUMN(R18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1760</v>
       </c>
       <c r="S18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S18)-ROW($C$5))*32+COLUMN(S18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0B82</v>
       </c>
       <c r="T18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T18)-ROW($C$5))*32+COLUMN(T18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0750</v>
       </c>
       <c r="U18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U18)-ROW($C$5))*32+COLUMN(U18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>039E</v>
       </c>
       <c r="V18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V18)-ROW($C$5))*32+COLUMN(V18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1000</v>
       </c>
       <c r="W18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W18)-ROW($C$5))*32+COLUMN(W18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0F82</v>
       </c>
       <c r="X18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X18)-ROW($C$5))*32+COLUMN(X18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0B80</v>
       </c>
       <c r="Y18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y18)-ROW($C$5))*32+COLUMN(Y18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FCAE</v>
       </c>
       <c r="Z18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z18)-ROW($C$5))*32+COLUMN(Z18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>1080</v>
       </c>
       <c r="AA18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA18)-ROW($C$5))*32+COLUMN(AA18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0BD4</v>
       </c>
       <c r="AB18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB18)-ROW($C$5))*32+COLUMN(AB18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0470</v>
       </c>
       <c r="AC18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC18)-ROW($C$5))*32+COLUMN(AC18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FBCE</v>
       </c>
       <c r="AD18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD18)-ROW($C$5))*32+COLUMN(AD18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0C92</v>
       </c>
       <c r="AE18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE18)-ROW($C$5))*32+COLUMN(AE18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0832</v>
       </c>
       <c r="AF18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF18)-ROW($C$5))*32+COLUMN(AF18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>07E0</v>
       </c>
       <c r="AG18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG18)-ROW($C$5))*32+COLUMN(AG18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F7FE</v>
       </c>
       <c r="AH18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH18)-ROW($C$5))*32+COLUMN(AH18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0CA2</v>
       </c>
     </row>
@@ -24337,131 +24486,131 @@
         <v>656</v>
       </c>
       <c r="C19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C19)-ROW($C$5))*32+COLUMN(C19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0010</v>
       </c>
       <c r="D19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D19)-ROW($C$5))*32+COLUMN(D19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0380</v>
       </c>
       <c r="E19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E19)-ROW($C$5))*32+COLUMN(E19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>13D0</v>
       </c>
       <c r="F19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F19)-ROW($C$5))*32+COLUMN(F19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F7A0</v>
       </c>
       <c r="G19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G19)-ROW($C$5))*32+COLUMN(G19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FFBE</v>
       </c>
       <c r="H19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H19)-ROW($C$5))*32+COLUMN(H19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0052</v>
       </c>
       <c r="I19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I19)-ROW($C$5))*32+COLUMN(I19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1380</v>
       </c>
       <c r="J19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J19)-ROW($C$5))*32+COLUMN(J19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F770</v>
       </c>
       <c r="K19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K19)-ROW($C$5))*32+COLUMN(K19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FF70</v>
       </c>
       <c r="L19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L19)-ROW($C$5))*32+COLUMN(L19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FFA0</v>
       </c>
       <c r="M19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M19)-ROW($C$5))*32+COLUMN(M19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0FC0</v>
       </c>
       <c r="N19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N19)-ROW($C$5))*32+COLUMN(N19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F3BE</v>
       </c>
       <c r="O19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O19)-ROW($C$5))*32+COLUMN(O19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0340</v>
       </c>
       <c r="P19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P19)-ROW($C$5))*32+COLUMN(P19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FF60</v>
       </c>
       <c r="Q19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q19)-ROW($C$5))*32+COLUMN(Q19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0FC0</v>
       </c>
       <c r="R19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R19)-ROW($C$5))*32+COLUMN(R19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F370</v>
       </c>
       <c r="S19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S19)-ROW($C$5))*32+COLUMN(S19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FB30</v>
       </c>
       <c r="T19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T19)-ROW($C$5))*32+COLUMN(T19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FB80</v>
       </c>
       <c r="U19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U19)-ROW($C$5))*32+COLUMN(U19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0C10</v>
       </c>
       <c r="V19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V19)-ROW($C$5))*32+COLUMN(V19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>E40E</v>
       </c>
       <c r="W19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W19)-ROW($C$5))*32+COLUMN(W19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FBA0</v>
       </c>
       <c r="X19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X19)-ROW($C$5))*32+COLUMN(X19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FBB0</v>
       </c>
       <c r="Y19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y19)-ROW($C$5))*32+COLUMN(Y19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0C42</v>
       </c>
       <c r="Z19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z19)-ROW($C$5))*32+COLUMN(Z19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>E860</v>
       </c>
       <c r="AA19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA19)-ROW($C$5))*32+COLUMN(AA19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FB92</v>
       </c>
       <c r="AB19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB19)-ROW($C$5))*32+COLUMN(AB19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F4A2</v>
       </c>
       <c r="AC19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC19)-ROW($C$5))*32+COLUMN(AC19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0B82</v>
       </c>
       <c r="AD19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD19)-ROW($C$5))*32+COLUMN(AD19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>E850</v>
       </c>
       <c r="AE19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE19)-ROW($C$5))*32+COLUMN(AE19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F832</v>
       </c>
       <c r="AF19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF19)-ROW($C$5))*32+COLUMN(AF19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FBA2</v>
       </c>
       <c r="AG19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG19)-ROW($C$5))*32+COLUMN(AG19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0002</v>
       </c>
       <c r="AH19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH19)-ROW($C$5))*32+COLUMN(AH19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>E470</v>
       </c>
     </row>
@@ -24471,131 +24620,131 @@
         <v>657</v>
       </c>
       <c r="C20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C20)-ROW($C$5))*32+COLUMN(C20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0022</v>
       </c>
       <c r="D20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D20)-ROW($C$5))*32+COLUMN(D20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F7A0</v>
       </c>
       <c r="E20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E20)-ROW($C$5))*32+COLUMN(E20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>EFFE</v>
       </c>
       <c r="F20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F20)-ROW($C$5))*32+COLUMN(F20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0BC0</v>
       </c>
       <c r="G20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G20)-ROW($C$5))*32+COLUMN(G20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>03D2</v>
       </c>
       <c r="H20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H20)-ROW($C$5))*32+COLUMN(H20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F860</v>
       </c>
       <c r="I20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I20)-ROW($C$5))*32+COLUMN(I20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F79E</v>
       </c>
       <c r="J20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J20)-ROW($C$5))*32+COLUMN(J20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0F92</v>
       </c>
       <c r="K20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K20)-ROW($C$5))*32+COLUMN(K20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0390</v>
       </c>
       <c r="L20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L20)-ROW($C$5))*32+COLUMN(L20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FFB0</v>
       </c>
       <c r="M20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M20)-ROW($C$5))*32+COLUMN(M20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F3FE</v>
       </c>
       <c r="N20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N20)-ROW($C$5))*32+COLUMN(N20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0FC0</v>
       </c>
       <c r="O20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O20)-ROW($C$5))*32+COLUMN(O20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0762</v>
       </c>
       <c r="P20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P20)-ROW($C$5))*32+COLUMN(P20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FF70</v>
       </c>
       <c r="Q20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q20)-ROW($C$5))*32+COLUMN(Q20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>EFFE</v>
       </c>
       <c r="R20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R20)-ROW($C$5))*32+COLUMN(R20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1380</v>
       </c>
       <c r="S20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S20)-ROW($C$5))*32+COLUMN(S20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0362</v>
       </c>
       <c r="T20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T20)-ROW($C$5))*32+COLUMN(T20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FFB0</v>
       </c>
       <c r="U20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U20)-ROW($C$5))*32+COLUMN(U20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F42E</v>
       </c>
       <c r="V20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V20)-ROW($C$5))*32+COLUMN(V20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0810</v>
       </c>
       <c r="W20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W20)-ROW($C$5))*32+COLUMN(W20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>07A2</v>
       </c>
       <c r="X20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X20)-ROW($C$5))*32+COLUMN(X20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>07C0</v>
       </c>
       <c r="Y20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y20)-ROW($C$5))*32+COLUMN(Y20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F87E</v>
       </c>
       <c r="Z20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z20)-ROW($C$5))*32+COLUMN(Z20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0C82</v>
       </c>
       <c r="AA20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA20)-ROW($C$5))*32+COLUMN(AA20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0B94</v>
       </c>
       <c r="AB20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB20)-ROW($C$5))*32+COLUMN(AB20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0490</v>
       </c>
       <c r="AC20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC20)-ROW($C$5))*32+COLUMN(AC20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FB90</v>
       </c>
       <c r="AD20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD20)-ROW($C$5))*32+COLUMN(AD20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>1062</v>
       </c>
       <c r="AE20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE20)-ROW($C$5))*32+COLUMN(AE20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0842</v>
       </c>
       <c r="AF20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF20)-ROW($C$5))*32+COLUMN(AF20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>07B0</v>
       </c>
       <c r="AG20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG20)-ROW($C$5))*32+COLUMN(AG20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>EC10</v>
       </c>
       <c r="AH20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH20)-ROW($C$5))*32+COLUMN(AH20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0C82</v>
       </c>
     </row>
@@ -24605,131 +24754,131 @@
         <v>658</v>
       </c>
       <c r="C21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C21)-ROW($C$5))*32+COLUMN(C21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0850</v>
       </c>
       <c r="D21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D21)-ROW($C$5))*32+COLUMN(D21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>13E2</v>
       </c>
       <c r="E21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E21)-ROW($C$5))*32+COLUMN(E21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>2360</v>
       </c>
       <c r="F21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F21)-ROW($C$5))*32+COLUMN(F21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0420</v>
       </c>
       <c r="G21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G21)-ROW($C$5))*32+COLUMN(G21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0460</v>
       </c>
       <c r="H21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H21)-ROW($C$5))*32+COLUMN(H21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>10B0</v>
       </c>
       <c r="I21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I21)-ROW($C$5))*32+COLUMN(I21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1FB0</v>
       </c>
       <c r="J21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J21)-ROW($C$5))*32+COLUMN(J21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>03E0</v>
       </c>
       <c r="K21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K21)-ROW($C$5))*32+COLUMN(K21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0B80</v>
       </c>
       <c r="L21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L21)-ROW($C$5))*32+COLUMN(L21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0BF0</v>
       </c>
       <c r="M21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M21)-ROW($C$5))*32+COLUMN(M21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1430</v>
       </c>
       <c r="N21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N21)-ROW($C$5))*32+COLUMN(N21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FC00</v>
       </c>
       <c r="O21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O21)-ROW($C$5))*32+COLUMN(O21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0F90</v>
       </c>
       <c r="P21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P21)-ROW($C$5))*32+COLUMN(P21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0BC2</v>
       </c>
       <c r="Q21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q21)-ROW($C$5))*32+COLUMN(Q21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1BA0</v>
       </c>
       <c r="R21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R21)-ROW($C$5))*32+COLUMN(R21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FFC0</v>
       </c>
       <c r="S21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S21)-ROW($C$5))*32+COLUMN(S21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>07C2</v>
       </c>
       <c r="T21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T21)-ROW($C$5))*32+COLUMN(T21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0B82</v>
       </c>
       <c r="U21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U21)-ROW($C$5))*32+COLUMN(U21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1BF0</v>
       </c>
       <c r="V21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V21)-ROW($C$5))*32+COLUMN(V21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F44E</v>
       </c>
       <c r="W21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W21)-ROW($C$5))*32+COLUMN(W21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0BB2</v>
       </c>
       <c r="X21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X21)-ROW($C$5))*32+COLUMN(X21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0FD2</v>
       </c>
       <c r="Y21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y21)-ROW($C$5))*32+COLUMN(Y21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>14C2</v>
       </c>
       <c r="Z21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z21)-ROW($C$5))*32+COLUMN(Z21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F8A0</v>
       </c>
       <c r="AA21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA21)-ROW($C$5))*32+COLUMN(AA21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0792</v>
       </c>
       <c r="AB21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB21)-ROW($C$5))*32+COLUMN(AB21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0852</v>
       </c>
       <c r="AC21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC21)-ROW($C$5))*32+COLUMN(AC21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>13E2</v>
       </c>
       <c r="AD21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD21)-ROW($C$5))*32+COLUMN(AD21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F850</v>
       </c>
       <c r="AE21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE21)-ROW($C$5))*32+COLUMN(AE21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>00A0</v>
       </c>
       <c r="AF21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF21)-ROW($C$5))*32+COLUMN(AF21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0032</v>
       </c>
       <c r="AG21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG21)-ROW($C$5))*32+COLUMN(AG21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0C22</v>
       </c>
       <c r="AH21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH21)-ROW($C$5))*32+COLUMN(AH21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F0D0</v>
       </c>
     </row>
@@ -24739,131 +24888,131 @@
         <v>659</v>
       </c>
       <c r="C22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C22)-ROW($C$5))*32+COLUMN(C22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F452</v>
       </c>
       <c r="D22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D22)-ROW($C$5))*32+COLUMN(D22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>EFE0</v>
       </c>
       <c r="E22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E22)-ROW($C$5))*32+COLUMN(E22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>EF7E</v>
       </c>
       <c r="F22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F22)-ROW($C$5))*32+COLUMN(F22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FC32</v>
       </c>
       <c r="G22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G22)-ROW($C$5))*32+COLUMN(G22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F072</v>
       </c>
       <c r="H22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H22)-ROW($C$5))*32+COLUMN(H22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F4C0</v>
       </c>
       <c r="I22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I22)-ROW($C$5))*32+COLUMN(I22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>EBCE</v>
       </c>
       <c r="J22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J22)-ROW($C$5))*32+COLUMN(J22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>03F0</v>
       </c>
       <c r="K22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K22)-ROW($C$5))*32+COLUMN(K22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FBA2</v>
       </c>
       <c r="L22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L22)-ROW($C$5))*32+COLUMN(L22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F400</v>
       </c>
       <c r="M22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M22)-ROW($C$5))*32+COLUMN(M22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>E45E</v>
       </c>
       <c r="N22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N22)-ROW($C$5))*32+COLUMN(N22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0410</v>
       </c>
       <c r="O22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O22)-ROW($C$5))*32+COLUMN(O22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FFA2</v>
       </c>
       <c r="P22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P22)-ROW($C$5))*32+COLUMN(P22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F7D0</v>
       </c>
       <c r="Q22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q22)-ROW($C$5))*32+COLUMN(Q22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>EBBE</v>
       </c>
       <c r="R22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R22)-ROW($C$5))*32+COLUMN(R22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0BD0</v>
       </c>
       <c r="S22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S22)-ROW($C$5))*32+COLUMN(S22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FBC2</v>
       </c>
       <c r="T22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T22)-ROW($C$5))*32+COLUMN(T22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FB80</v>
       </c>
       <c r="U22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U22)-ROW($C$5))*32+COLUMN(U22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F00E</v>
       </c>
       <c r="V22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V22)-ROW($C$5))*32+COLUMN(V22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0050</v>
       </c>
       <c r="W22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W22)-ROW($C$5))*32+COLUMN(W22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>03D2</v>
       </c>
       <c r="X22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X22)-ROW($C$5))*32+COLUMN(X22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>03D0</v>
       </c>
       <c r="Y22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y22)-ROW($C$5))*32+COLUMN(Y22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F0E0</v>
       </c>
       <c r="Z22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z22)-ROW($C$5))*32+COLUMN(Z22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0CA0</v>
       </c>
       <c r="AA22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA22)-ROW($C$5))*32+COLUMN(AA22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0384</v>
       </c>
       <c r="AB22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB22)-ROW($C$5))*32+COLUMN(AB22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0440</v>
       </c>
       <c r="AC22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC22)-ROW($C$5))*32+COLUMN(AC22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F3EE</v>
       </c>
       <c r="AD22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD22)-ROW($C$5))*32+COLUMN(AD22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0C52</v>
       </c>
       <c r="AE22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE22)-ROW($C$5))*32+COLUMN(AE22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>00A2</v>
       </c>
       <c r="AF22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF22)-ROW($C$5))*32+COLUMN(AF22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0030</v>
       </c>
       <c r="AG22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG22)-ROW($C$5))*32+COLUMN(AG22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>EC20</v>
       </c>
       <c r="AH22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH22)-ROW($C$5))*32+COLUMN(AH22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>04C0</v>
       </c>
     </row>
@@ -24873,131 +25022,131 @@
         <v>660</v>
       </c>
       <c r="C23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C23)-ROW($C$5))*32+COLUMN(C23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1022</v>
       </c>
       <c r="D23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D23)-ROW($C$5))*32+COLUMN(D23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0FD2</v>
       </c>
       <c r="E23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E23)-ROW($C$5))*32+COLUMN(E23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1F80</v>
       </c>
       <c r="F23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F23)-ROW($C$5))*32+COLUMN(F23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>03F0</v>
       </c>
       <c r="G23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G23)-ROW($C$5))*32+COLUMN(G23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0830</v>
       </c>
       <c r="H23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H23)-ROW($C$5))*32+COLUMN(H23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0C82</v>
       </c>
       <c r="I23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I23)-ROW($C$5))*32+COLUMN(I23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>17E0</v>
       </c>
       <c r="J23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J23)-ROW($C$5))*32+COLUMN(J23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FFB0</v>
       </c>
       <c r="K23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K23)-ROW($C$5))*32+COLUMN(K23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0410</v>
       </c>
       <c r="L23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L23)-ROW($C$5))*32+COLUMN(L23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0432</v>
       </c>
       <c r="M23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M23)-ROW($C$5))*32+COLUMN(M23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0870</v>
       </c>
       <c r="N23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N23)-ROW($C$5))*32+COLUMN(N23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F48E</v>
       </c>
       <c r="O23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O23)-ROW($C$5))*32+COLUMN(O23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0BD0</v>
       </c>
       <c r="P23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P23)-ROW($C$5))*32+COLUMN(P23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>07B2</v>
       </c>
       <c r="Q23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q23)-ROW($C$5))*32+COLUMN(Q23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0F90</v>
       </c>
       <c r="R23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R23)-ROW($C$5))*32+COLUMN(R23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FBB0</v>
       </c>
       <c r="S23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S23)-ROW($C$5))*32+COLUMN(S23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FFF0</v>
       </c>
       <c r="T23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T23)-ROW($C$5))*32+COLUMN(T23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>07A2</v>
       </c>
       <c r="U23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U23)-ROW($C$5))*32+COLUMN(U23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1410</v>
       </c>
       <c r="V23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V23)-ROW($C$5))*32+COLUMN(V23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F410</v>
       </c>
       <c r="W23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W23)-ROW($C$5))*32+COLUMN(W23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0022</v>
       </c>
       <c r="X23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X23)-ROW($C$5))*32+COLUMN(X23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0BC2</v>
       </c>
       <c r="Y23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y23)-ROW($C$5))*32+COLUMN(Y23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0CE0</v>
       </c>
       <c r="Z23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z23)-ROW($C$5))*32+COLUMN(Z23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F850</v>
       </c>
       <c r="AA23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA23)-ROW($C$5))*32+COLUMN(AA23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FFB2</v>
       </c>
       <c r="AB23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB23)-ROW($C$5))*32+COLUMN(AB23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0490</v>
       </c>
       <c r="AC23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC23)-ROW($C$5))*32+COLUMN(AC23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0BC0</v>
       </c>
       <c r="AD23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD23)-ROW($C$5))*32+COLUMN(AD23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>ECC0</v>
       </c>
       <c r="AE23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE23)-ROW($C$5))*32+COLUMN(AE23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FC70</v>
       </c>
       <c r="AF23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF23)-ROW($C$5))*32+COLUMN(AF23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0012</v>
       </c>
       <c r="AG23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG23)-ROW($C$5))*32+COLUMN(AG23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0400</v>
       </c>
       <c r="AH23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH23)-ROW($C$5))*32+COLUMN(AH23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F0B2</v>
       </c>
     </row>
@@ -25007,131 +25156,131 @@
         <v>661</v>
       </c>
       <c r="C24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C24)-ROW($C$5))*32+COLUMN(C24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0402</v>
       </c>
       <c r="D24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D24)-ROW($C$5))*32+COLUMN(D24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F7D0</v>
       </c>
       <c r="E24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E24)-ROW($C$5))*32+COLUMN(E24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F37E</v>
       </c>
       <c r="F24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F24)-ROW($C$5))*32+COLUMN(F24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0BF2</v>
       </c>
       <c r="G24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G24)-ROW($C$5))*32+COLUMN(G24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0022</v>
       </c>
       <c r="H24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H24)-ROW($C$5))*32+COLUMN(H24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FC90</v>
       </c>
       <c r="I24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I24)-ROW($C$5))*32+COLUMN(I24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>EFFE</v>
       </c>
       <c r="J24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J24)-ROW($C$5))*32+COLUMN(J24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0FC2</v>
       </c>
       <c r="K24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K24)-ROW($C$5))*32+COLUMN(K24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FC12</v>
       </c>
       <c r="L24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L24)-ROW($C$5))*32+COLUMN(L24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F84E</v>
       </c>
       <c r="M24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M24)-ROW($C$5))*32+COLUMN(M24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>E87E</v>
       </c>
       <c r="N24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N24)-ROW($C$5))*32+COLUMN(N24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0480</v>
       </c>
       <c r="O24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O24)-ROW($C$5))*32+COLUMN(O24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>07E2</v>
       </c>
       <c r="P24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P24)-ROW($C$5))*32+COLUMN(P24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FFB0</v>
       </c>
       <c r="Q24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q24)-ROW($C$5))*32+COLUMN(Q24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F7AE</v>
       </c>
       <c r="R24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R24)-ROW($C$5))*32+COLUMN(R24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0FC0</v>
       </c>
       <c r="S24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S24)-ROW($C$5))*32+COLUMN(S24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0002</v>
       </c>
       <c r="T24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T24)-ROW($C$5))*32+COLUMN(T24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>07A0</v>
       </c>
       <c r="U24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U24)-ROW($C$5))*32+COLUMN(U24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F81E</v>
       </c>
       <c r="V24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V24)-ROW($C$5))*32+COLUMN(V24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1002</v>
       </c>
       <c r="W24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W24)-ROW($C$5))*32+COLUMN(W24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0422</v>
       </c>
       <c r="X24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X24)-ROW($C$5))*32+COLUMN(X24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0FD0</v>
       </c>
       <c r="Y24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y24)-ROW($C$5))*32+COLUMN(Y24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F8CE</v>
       </c>
       <c r="Z24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z24)-ROW($C$5))*32+COLUMN(Z24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>1842</v>
       </c>
       <c r="AA24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA24)-ROW($C$5))*32+COLUMN(AA24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>07A4</v>
       </c>
       <c r="AB24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB24)-ROW($C$5))*32+COLUMN(AB24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0880</v>
       </c>
       <c r="AC24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC24)-ROW($C$5))*32+COLUMN(AC24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FBB0</v>
       </c>
       <c r="AD24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD24)-ROW($C$5))*32+COLUMN(AD24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0CB0</v>
       </c>
       <c r="AE24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE24)-ROW($C$5))*32+COLUMN(AE24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0C62</v>
       </c>
       <c r="AF24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF24)-ROW($C$5))*32+COLUMN(AF24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0BF0</v>
       </c>
       <c r="AG24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG24)-ROW($C$5))*32+COLUMN(AG24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FBF0</v>
       </c>
       <c r="AH24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH24)-ROW($C$5))*32+COLUMN(AH24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>10A0</v>
       </c>
     </row>
@@ -25141,131 +25290,131 @@
         <v>662</v>
       </c>
       <c r="C25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C25)-ROW($C$5))*32+COLUMN(C25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ref="C25:L30" ca="1" si="6">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C25)-ROW($C$5))*32+COLUMN(C25)-COLUMN($C$5),,,"Input data"))</f>
         <v>F030</v>
       </c>
       <c r="D25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D25)-ROW($C$5))*32+COLUMN(D25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>07D2</v>
       </c>
       <c r="E25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E25)-ROW($C$5))*32+COLUMN(E25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0BE0</v>
       </c>
       <c r="F25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F25)-ROW($C$5))*32+COLUMN(F25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F800</v>
       </c>
       <c r="G25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G25)-ROW($C$5))*32+COLUMN(G25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>ECA0</v>
       </c>
       <c r="H25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H25)-ROW($C$5))*32+COLUMN(H25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0482</v>
       </c>
       <c r="I25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I25)-ROW($C$5))*32+COLUMN(I25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0830</v>
       </c>
       <c r="J25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J25)-ROW($C$5))*32+COLUMN(J25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>FBE0</v>
       </c>
       <c r="K25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K25)-ROW($C$5))*32+COLUMN(K25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F040</v>
       </c>
       <c r="L25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L25)-ROW($C$5))*32+COLUMN(L25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>FC80</v>
       </c>
       <c r="M25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M25)-ROW($C$5))*32+COLUMN(M25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ref="M25:V30" ca="1" si="7">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M25)-ROW($C$5))*32+COLUMN(M25)-COLUMN($C$5),,,"Input data"))</f>
         <v>0810</v>
       </c>
       <c r="N25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N25)-ROW($C$5))*32+COLUMN(N25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F030</v>
       </c>
       <c r="O25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O25)-ROW($C$5))*32+COLUMN(O25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F410</v>
       </c>
       <c r="P25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P25)-ROW($C$5))*32+COLUMN(P25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F830</v>
       </c>
       <c r="Q25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q25)-ROW($C$5))*32+COLUMN(Q25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0BA0</v>
       </c>
       <c r="R25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R25)-ROW($C$5))*32+COLUMN(R25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F7A0</v>
       </c>
       <c r="S25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S25)-ROW($C$5))*32+COLUMN(S25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F3D2</v>
       </c>
       <c r="T25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T25)-ROW($C$5))*32+COLUMN(T25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>FFF2</v>
       </c>
       <c r="U25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U25)-ROW($C$5))*32+COLUMN(U25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0840</v>
       </c>
       <c r="V25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V25)-ROW($C$5))*32+COLUMN(V25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>EFF0</v>
       </c>
       <c r="W25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W25)-ROW($C$5))*32+COLUMN(W25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ref="W25:AH30" ca="1" si="8">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W25)-ROW($C$5))*32+COLUMN(W25)-COLUMN($C$5),,,"Input data"))</f>
         <v>F400</v>
       </c>
       <c r="X25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X25)-ROW($C$5))*32+COLUMN(X25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>03B2</v>
       </c>
       <c r="Y25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y25)-ROW($C$5))*32+COLUMN(Y25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0872</v>
       </c>
       <c r="Z25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z25)-ROW($C$5))*32+COLUMN(Z25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>F030</v>
       </c>
       <c r="AA25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA25)-ROW($C$5))*32+COLUMN(AA25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>EFB2</v>
       </c>
       <c r="AB25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB25)-ROW($C$5))*32+COLUMN(AB25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0042</v>
       </c>
       <c r="AC25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC25)-ROW($C$5))*32+COLUMN(AC25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>03B2</v>
       </c>
       <c r="AD25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD25)-ROW($C$5))*32+COLUMN(AD25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>EC40</v>
       </c>
       <c r="AE25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE25)-ROW($C$5))*32+COLUMN(AE25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FFE0</v>
       </c>
       <c r="AF25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF25)-ROW($C$5))*32+COLUMN(AF25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FFE2</v>
       </c>
       <c r="AG25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG25)-ROW($C$5))*32+COLUMN(AG25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0012</v>
       </c>
       <c r="AH25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH25)-ROW($C$5))*32+COLUMN(AH25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>F420</v>
       </c>
     </row>
@@ -25275,131 +25424,131 @@
         <v>663</v>
       </c>
       <c r="C26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C26)-ROW($C$5))*32+COLUMN(C26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F422</v>
       </c>
       <c r="D26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D26)-ROW($C$5))*32+COLUMN(D26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F7B0</v>
       </c>
       <c r="E26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E26)-ROW($C$5))*32+COLUMN(E26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>E7CE</v>
       </c>
       <c r="F26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F26)-ROW($C$5))*32+COLUMN(F26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0BD2</v>
       </c>
       <c r="G26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G26)-ROW($C$5))*32+COLUMN(G26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F080</v>
       </c>
       <c r="H26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H26)-ROW($C$5))*32+COLUMN(H26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0070</v>
       </c>
       <c r="I26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I26)-ROW($C$5))*32+COLUMN(I26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>EC2E</v>
       </c>
       <c r="J26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J26)-ROW($C$5))*32+COLUMN(J26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0FE2</v>
       </c>
       <c r="K26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K26)-ROW($C$5))*32+COLUMN(K26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F850</v>
       </c>
       <c r="L26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L26)-ROW($C$5))*32+COLUMN(L26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0070</v>
       </c>
       <c r="M26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M26)-ROW($C$5))*32+COLUMN(M26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F00E</v>
       </c>
       <c r="N26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N26)-ROW($C$5))*32+COLUMN(N26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0C42</v>
       </c>
       <c r="O26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O26)-ROW($C$5))*32+COLUMN(O26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0020</v>
       </c>
       <c r="P26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P26)-ROW($C$5))*32+COLUMN(P26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0030</v>
       </c>
       <c r="Q26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q26)-ROW($C$5))*32+COLUMN(Q26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F7AE</v>
       </c>
       <c r="R26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R26)-ROW($C$5))*32+COLUMN(R26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>17B2</v>
       </c>
       <c r="S26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S26)-ROW($C$5))*32+COLUMN(S26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>03D2</v>
       </c>
       <c r="T26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T26)-ROW($C$5))*32+COLUMN(T26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0400</v>
       </c>
       <c r="U26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U26)-ROW($C$5))*32+COLUMN(U26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F84E</v>
       </c>
       <c r="V26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V26)-ROW($C$5))*32+COLUMN(V26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>17F0</v>
       </c>
       <c r="W26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W26)-ROW($C$5))*32+COLUMN(W26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0BE2</v>
       </c>
       <c r="X26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X26)-ROW($C$5))*32+COLUMN(X26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>13A0</v>
       </c>
       <c r="Y26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y26)-ROW($C$5))*32+COLUMN(Y26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FC4E</v>
       </c>
       <c r="Z26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z26)-ROW($C$5))*32+COLUMN(Z26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1820</v>
       </c>
       <c r="AA26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA26)-ROW($C$5))*32+COLUMN(AA26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0792</v>
       </c>
       <c r="AB26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB26)-ROW($C$5))*32+COLUMN(AB26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1020</v>
       </c>
       <c r="AC26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC26)-ROW($C$5))*32+COLUMN(AC26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FB9E</v>
       </c>
       <c r="AD26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD26)-ROW($C$5))*32+COLUMN(AD26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1C10</v>
       </c>
       <c r="AE26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE26)-ROW($C$5))*32+COLUMN(AE26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1BC2</v>
       </c>
       <c r="AF26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF26)-ROW($C$5))*32+COLUMN(AF26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>13C0</v>
       </c>
       <c r="AG26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG26)-ROW($C$5))*32+COLUMN(AG26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FBE0</v>
       </c>
       <c r="AH26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH26)-ROW($C$5))*32+COLUMN(AH26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>2002</v>
       </c>
     </row>
@@ -25409,131 +25558,131 @@
         <v>664</v>
       </c>
       <c r="C27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C27)-ROW($C$5))*32+COLUMN(C27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F040</v>
       </c>
       <c r="D27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D27)-ROW($C$5))*32+COLUMN(D27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>13A2</v>
       </c>
       <c r="E27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E27)-ROW($C$5))*32+COLUMN(E27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0F80</v>
       </c>
       <c r="F27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F27)-ROW($C$5))*32+COLUMN(F27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>FC30</v>
       </c>
       <c r="G27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G27)-ROW($C$5))*32+COLUMN(G27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F46E</v>
       </c>
       <c r="H27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H27)-ROW($C$5))*32+COLUMN(H27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0CC2</v>
       </c>
       <c r="I27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I27)-ROW($C$5))*32+COLUMN(I27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>17B2</v>
       </c>
       <c r="J27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J27)-ROW($C$5))*32+COLUMN(J27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0010</v>
       </c>
       <c r="K27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K27)-ROW($C$5))*32+COLUMN(K27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>FC10</v>
       </c>
       <c r="L27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L27)-ROW($C$5))*32+COLUMN(L27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0872</v>
       </c>
       <c r="M27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M27)-ROW($C$5))*32+COLUMN(M27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>1000</v>
       </c>
       <c r="N27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N27)-ROW($C$5))*32+COLUMN(N27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F8B0</v>
       </c>
       <c r="O27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O27)-ROW($C$5))*32+COLUMN(O27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>07BE</v>
       </c>
       <c r="P27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P27)-ROW($C$5))*32+COLUMN(P27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0BE2</v>
       </c>
       <c r="Q27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q27)-ROW($C$5))*32+COLUMN(Q27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>13B0</v>
       </c>
       <c r="R27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R27)-ROW($C$5))*32+COLUMN(R27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>FFE0</v>
       </c>
       <c r="S27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S27)-ROW($C$5))*32+COLUMN(S27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F410</v>
       </c>
       <c r="T27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T27)-ROW($C$5))*32+COLUMN(T27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0450</v>
       </c>
       <c r="U27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U27)-ROW($C$5))*32+COLUMN(U27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0C70</v>
       </c>
       <c r="V27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V27)-ROW($C$5))*32+COLUMN(V27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F420</v>
       </c>
       <c r="W27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W27)-ROW($C$5))*32+COLUMN(W27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>03C0</v>
       </c>
       <c r="X27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X27)-ROW($C$5))*32+COLUMN(X27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0F82</v>
       </c>
       <c r="Y27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y27)-ROW($C$5))*32+COLUMN(Y27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1060</v>
       </c>
       <c r="Z27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z27)-ROW($C$5))*32+COLUMN(Z27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FFE0</v>
       </c>
       <c r="AA27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA27)-ROW($C$5))*32+COLUMN(AA27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FB70</v>
       </c>
       <c r="AB27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB27)-ROW($C$5))*32+COLUMN(AB27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>13D2</v>
       </c>
       <c r="AC27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC27)-ROW($C$5))*32+COLUMN(AC27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0F90</v>
       </c>
       <c r="AD27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD27)-ROW($C$5))*32+COLUMN(AD27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>F820</v>
       </c>
       <c r="AE27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE27)-ROW($C$5))*32+COLUMN(AE27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FC40</v>
       </c>
       <c r="AF27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF27)-ROW($C$5))*32+COLUMN(AF27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0FA2</v>
       </c>
       <c r="AG27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG27)-ROW($C$5))*32+COLUMN(AG27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0BE2</v>
       </c>
       <c r="AH27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH27)-ROW($C$5))*32+COLUMN(AH27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FC60</v>
       </c>
     </row>
@@ -25543,131 +25692,131 @@
         <v>665</v>
       </c>
       <c r="C28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C28)-ROW($C$5))*32+COLUMN(C28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F012</v>
       </c>
       <c r="D28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D28)-ROW($C$5))*32+COLUMN(D28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>FB80</v>
       </c>
       <c r="E28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E28)-ROW($C$5))*32+COLUMN(E28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>EB5E</v>
       </c>
       <c r="F28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F28)-ROW($C$5))*32+COLUMN(F28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0802</v>
       </c>
       <c r="G28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G28)-ROW($C$5))*32+COLUMN(G28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F420</v>
       </c>
       <c r="H28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H28)-ROW($C$5))*32+COLUMN(H28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0090</v>
       </c>
       <c r="I28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I28)-ROW($C$5))*32+COLUMN(I28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F78E</v>
       </c>
       <c r="J28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J28)-ROW($C$5))*32+COLUMN(J28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>13E2</v>
       </c>
       <c r="K28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K28)-ROW($C$5))*32+COLUMN(K28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>FC02</v>
       </c>
       <c r="L28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L28)-ROW($C$5))*32+COLUMN(L28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0060</v>
       </c>
       <c r="M28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M28)-ROW($C$5))*32+COLUMN(M28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F40E</v>
       </c>
       <c r="N28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N28)-ROW($C$5))*32+COLUMN(N28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>1090</v>
       </c>
       <c r="O28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O28)-ROW($C$5))*32+COLUMN(O28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0F90</v>
       </c>
       <c r="P28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P28)-ROW($C$5))*32+COLUMN(P28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0BD0</v>
       </c>
       <c r="Q28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q28)-ROW($C$5))*32+COLUMN(Q28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>FBAE</v>
       </c>
       <c r="R28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R28)-ROW($C$5))*32+COLUMN(R28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>1FD2</v>
       </c>
       <c r="S28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S28)-ROW($C$5))*32+COLUMN(S28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0002</v>
       </c>
       <c r="T28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T28)-ROW($C$5))*32+COLUMN(T28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0820</v>
       </c>
       <c r="U28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U28)-ROW($C$5))*32+COLUMN(U28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F85E</v>
       </c>
       <c r="V28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V28)-ROW($C$5))*32+COLUMN(V28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>1800</v>
       </c>
       <c r="W28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W28)-ROW($C$5))*32+COLUMN(W28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0F82</v>
       </c>
       <c r="X28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X28)-ROW($C$5))*32+COLUMN(X28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1B60</v>
       </c>
       <c r="Y28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y28)-ROW($C$5))*32+COLUMN(Y28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FC3E</v>
       </c>
       <c r="Z28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z28)-ROW($C$5))*32+COLUMN(Z28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>23C2</v>
       </c>
       <c r="AA28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA28)-ROW($C$5))*32+COLUMN(AA28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0B42</v>
       </c>
       <c r="AB28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB28)-ROW($C$5))*32+COLUMN(AB28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1BA0</v>
       </c>
       <c r="AC28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC28)-ROW($C$5))*32+COLUMN(AC28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FF7E</v>
       </c>
       <c r="AD28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD28)-ROW($C$5))*32+COLUMN(AD28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>27E0</v>
       </c>
       <c r="AE28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE28)-ROW($C$5))*32+COLUMN(AE28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1012</v>
       </c>
       <c r="AF28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF28)-ROW($C$5))*32+COLUMN(AF28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1B70</v>
       </c>
       <c r="AG28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG28)-ROW($C$5))*32+COLUMN(AG28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FFC0</v>
       </c>
       <c r="AH28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH28)-ROW($C$5))*32+COLUMN(AH28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>2040</v>
       </c>
     </row>
@@ -25677,131 +25826,131 @@
         <v>666</v>
       </c>
       <c r="C29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C29)-ROW($C$5))*32+COLUMN(C29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>FC70</v>
       </c>
       <c r="D29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D29)-ROW($C$5))*32+COLUMN(D29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>1BA2</v>
       </c>
       <c r="E29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E29)-ROW($C$5))*32+COLUMN(E29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0FA0</v>
       </c>
       <c r="F29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F29)-ROW($C$5))*32+COLUMN(F29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0BA0</v>
       </c>
       <c r="G29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G29)-ROW($C$5))*32+COLUMN(G29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0002</v>
       </c>
       <c r="H29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H29)-ROW($C$5))*32+COLUMN(H29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>1432</v>
       </c>
       <c r="I29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I29)-ROW($C$5))*32+COLUMN(I29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0FE0</v>
       </c>
       <c r="J29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J29)-ROW($C$5))*32+COLUMN(J29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0010</v>
       </c>
       <c r="K29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K29)-ROW($C$5))*32+COLUMN(K29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F83E</v>
       </c>
       <c r="L29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L29)-ROW($C$5))*32+COLUMN(L29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>13E0</v>
       </c>
       <c r="M29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M29)-ROW($C$5))*32+COLUMN(M29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>085E</v>
       </c>
       <c r="N29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N29)-ROW($C$5))*32+COLUMN(N29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>07E0</v>
       </c>
       <c r="O29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O29)-ROW($C$5))*32+COLUMN(O29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>005E</v>
       </c>
       <c r="P29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P29)-ROW($C$5))*32+COLUMN(P29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0842</v>
       </c>
       <c r="Q29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q29)-ROW($C$5))*32+COLUMN(Q29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0FEE</v>
       </c>
       <c r="R29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R29)-ROW($C$5))*32+COLUMN(R29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>03D0</v>
       </c>
       <c r="S29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S29)-ROW($C$5))*32+COLUMN(S29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>FC20</v>
       </c>
       <c r="T29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T29)-ROW($C$5))*32+COLUMN(T29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0FE2</v>
       </c>
       <c r="U29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U29)-ROW($C$5))*32+COLUMN(U29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>1400</v>
       </c>
       <c r="V29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V29)-ROW($C$5))*32+COLUMN(V29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0780</v>
       </c>
       <c r="W29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W29)-ROW($C$5))*32+COLUMN(W29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0B90</v>
       </c>
       <c r="X29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X29)-ROW($C$5))*32+COLUMN(X29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1772</v>
       </c>
       <c r="Y29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y29)-ROW($C$5))*32+COLUMN(Y29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1410</v>
       </c>
       <c r="Z29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z29)-ROW($C$5))*32+COLUMN(Z29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>07B0</v>
       </c>
       <c r="AA29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA29)-ROW($C$5))*32+COLUMN(AA29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FB10</v>
       </c>
       <c r="AB29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB29)-ROW($C$5))*32+COLUMN(AB29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>17F2</v>
       </c>
       <c r="AC29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC29)-ROW($C$5))*32+COLUMN(AC29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0B20</v>
       </c>
       <c r="AD29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD29)-ROW($C$5))*32+COLUMN(AD29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>03F0</v>
       </c>
       <c r="AE29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE29)-ROW($C$5))*32+COLUMN(AE29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FC1E</v>
       </c>
       <c r="AF29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF29)-ROW($C$5))*32+COLUMN(AF29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>17B2</v>
       </c>
       <c r="AG29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG29)-ROW($C$5))*32+COLUMN(AG29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>07CE</v>
       </c>
       <c r="AH29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH29)-ROW($C$5))*32+COLUMN(AH29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0830</v>
       </c>
     </row>
@@ -25811,131 +25960,131 @@
         <v>667</v>
       </c>
       <c r="C30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C30)-ROW($C$5))*32+COLUMN(C30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>E050</v>
       </c>
       <c r="D30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D30)-ROW($C$5))*32+COLUMN(D30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>EF80</v>
       </c>
       <c r="E30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E30)-ROW($C$5))*32+COLUMN(E30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>D38E</v>
       </c>
       <c r="F30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F30)-ROW($C$5))*32+COLUMN(F30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0382</v>
       </c>
       <c r="G30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G30)-ROW($C$5))*32+COLUMN(G30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>EBE0</v>
       </c>
       <c r="H30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H30)-ROW($C$5))*32+COLUMN(H30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F810</v>
       </c>
       <c r="I30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I30)-ROW($C$5))*32+COLUMN(I30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>DFBE</v>
       </c>
       <c r="J30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J30)-ROW($C$5))*32+COLUMN(J30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>07D0</v>
       </c>
       <c r="K30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K30)-ROW($C$5))*32+COLUMN(K30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>EC10</v>
       </c>
       <c r="L30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L30)-ROW($C$5))*32+COLUMN(L30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>FFC0</v>
       </c>
       <c r="M30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M30)-ROW($C$5))*32+COLUMN(M30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>E01E</v>
       </c>
       <c r="N30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N30)-ROW($C$5))*32+COLUMN(N30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0BB0</v>
       </c>
       <c r="O30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O30)-ROW($C$5))*32+COLUMN(O30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F820</v>
       </c>
       <c r="P30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P30)-ROW($C$5))*32+COLUMN(P30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F810</v>
       </c>
       <c r="Q30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q30)-ROW($C$5))*32+COLUMN(Q30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>EBBE</v>
       </c>
       <c r="R30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R30)-ROW($C$5))*32+COLUMN(R30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0BA0</v>
       </c>
       <c r="S30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S30)-ROW($C$5))*32+COLUMN(S30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>FBF0</v>
       </c>
       <c r="T30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T30)-ROW($C$5))*32+COLUMN(T30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>07A0</v>
       </c>
       <c r="U30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U30)-ROW($C$5))*32+COLUMN(U30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F3EE</v>
       </c>
       <c r="V30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V30)-ROW($C$5))*32+COLUMN(V30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>1B50</v>
       </c>
       <c r="W30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W30)-ROW($C$5))*32+COLUMN(W30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0752</v>
       </c>
       <c r="X30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X30)-ROW($C$5))*32+COLUMN(X30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0F30</v>
       </c>
       <c r="Y30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y30)-ROW($C$5))*32+COLUMN(Y30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>F7EE</v>
       </c>
       <c r="Z30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z30)-ROW($C$5))*32+COLUMN(Z30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1B80</v>
       </c>
       <c r="AA30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA30)-ROW($C$5))*32+COLUMN(AA30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>02F2</v>
       </c>
       <c r="AB30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB30)-ROW($C$5))*32+COLUMN(AB30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0FD0</v>
       </c>
       <c r="AC30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC30)-ROW($C$5))*32+COLUMN(AC30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>F70E</v>
       </c>
       <c r="AD30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD30)-ROW($C$5))*32+COLUMN(AD30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>13C0</v>
       </c>
       <c r="AE30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE30)-ROW($C$5))*32+COLUMN(AE30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0BE0</v>
       </c>
       <c r="AF30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF30)-ROW($C$5))*32+COLUMN(AF30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1390</v>
       </c>
       <c r="AG30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG30)-ROW($C$5))*32+COLUMN(AG30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>F79E</v>
       </c>
       <c r="AH30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH30)-ROW($C$5))*32+COLUMN(AH30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1C00</v>
       </c>
       <c r="AI30" s="3"/>
@@ -51242,8 +51391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AH114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52467,7 +52616,7 @@
         <v>FFA8</v>
       </c>
       <c r="K13" s="17" t="str">
-        <f t="shared" ref="K13:Z29" ca="1" si="2">INDIRECT(ADDRESS(ROW($B$4)+4,COLUMN($B$4)+(ROW(K13)-ROW($C$5))*32+COLUMN(K13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ref="K13:Z28" ca="1" si="2">INDIRECT(ADDRESS(ROW($B$4)+4,COLUMN($B$4)+(ROW(K13)-ROW($C$5))*32+COLUMN(K13)-COLUMN($C$5),,,"Input data"))</f>
         <v>FFBB</v>
       </c>
       <c r="L13" s="17" t="str">
@@ -52531,7 +52680,7 @@
         <v>FFA2</v>
       </c>
       <c r="AA13" s="17" t="str">
-        <f t="shared" ref="AA13:AH29" ca="1" si="3">INDIRECT(ADDRESS(ROW($B$4)+4,COLUMN($B$4)+(ROW(AA13)-ROW($C$5))*32+COLUMN(AA13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ref="AA13:AH28" ca="1" si="3">INDIRECT(ADDRESS(ROW($B$4)+4,COLUMN($B$4)+(ROW(AA13)-ROW($C$5))*32+COLUMN(AA13)-COLUMN($C$5),,,"Input data"))</f>
         <v>FFB4</v>
       </c>
       <c r="AB13" s="17" t="str">
@@ -54696,7 +54845,7 @@
         <v>4115</v>
       </c>
       <c r="C30" s="17" t="str">
-        <f t="shared" ref="C30:R31" ca="1" si="5">INDIRECT(ADDRESS(ROW($B$4)+4,COLUMN($B$4)+(ROW(C30)-ROW($C$5))*32+COLUMN(C30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ref="C30:I31" ca="1" si="5">INDIRECT(ADDRESS(ROW($B$4)+4,COLUMN($B$4)+(ROW(C30)-ROW($C$5))*32+COLUMN(C30)-COLUMN($C$5),,,"Input data"))</f>
         <v>0695</v>
       </c>
       <c r="D30" s="17" t="str">

</xml_diff>

<commit_message>
BadPixelsCorrection and LICENSE from upstream (#6)
* Added explanation on how to use the file

* Typos fixes

* Correction of bad pixels

* Using fabs() instead of abs()

* Adding Apache2 license to repo - So that everyone know this is actually open-source

* Updated examples to use BadPixelsCorrection
</commit_message>
<xml_diff>
--- a/MLX90640 example data.xlsx
+++ b/MLX90640 example data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="27795" windowHeight="14115" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="27795" windowHeight="14055"/>
   </bookViews>
   <sheets>
     <sheet name="Input data" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10432" uniqueCount="4736">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10446" uniqueCount="4748">
   <si>
     <t>00AE</t>
   </si>
@@ -14271,12 +14271,72 @@
   <si>
     <t>This sheet copntains the calculated To based on the data from sheet 'Input data'</t>
   </si>
+  <si>
+    <t>1. Load the sample EEPROM data into the MCU memory allocated for it.</t>
+  </si>
+  <si>
+    <t>3. Download the calculated parameters and compare to the ones in the sample data file.</t>
+  </si>
+  <si>
+    <t>4. Load the sample frame 0 data into the MCU memory allocated for the frame data and call</t>
+  </si>
+  <si>
+    <t>5. Download the calculated frame temperatures and compare with the ones in the sample data file</t>
+  </si>
+  <si>
+    <t>6. Load the sample frame 1 data into the MCU memory allocated for the frame data and call</t>
+  </si>
+  <si>
+    <t>7. Download the calculated frame temperatures and compare with the ones in the sample data file</t>
+  </si>
+  <si>
+    <t>Verification flow</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. Call the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MLX90640_ExtractParameters(pEEPROM, pParams)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> function</t>
+    </r>
+  </si>
+  <si>
+    <t>tr = MLX90640_GetTa(pFrame, pParams) - 8;</t>
+  </si>
+  <si>
+    <t>MLX90640_CalculateTo(pFrame, pParams, 1.0, tr, pTo);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If all the values you get are the same as the ones in the sample data file, the driver has compiled correctly and all the addressing is intact. </t>
+  </si>
+  <si>
+    <t>All that is left to do is to simply get live data from the sensor and put it in the appropriate memory location.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -14293,6 +14353,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
@@ -14342,7 +14411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -14385,6 +14454,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14686,10 +14761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AFC18"/>
+  <dimension ref="B1:AFC34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22312,8 +22387,82 @@
       <c r="M18" s="18"/>
       <c r="N18" s="18"/>
     </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>4742</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="20" t="s">
+        <v>4736</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="20" t="s">
+        <v>4743</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B23" s="20" t="s">
+        <v>4737</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="20" t="s">
+        <v>4738</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="21" t="s">
+        <v>4744</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="21" t="s">
+        <v>4745</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="20" t="s">
+        <v>4739</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="20" t="s">
+        <v>4740</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B29" s="21" t="s">
+        <v>4744</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B30" s="21" t="s">
+        <v>4745</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B31" s="20" t="s">
+        <v>4741</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B32"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>4746</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
+        <v>4747</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -22322,7 +22471,7 @@
   <dimension ref="A2:AI3153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22460,131 +22609,131 @@
         <v>642</v>
       </c>
       <c r="C5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C5)-ROW($C$5))*32+COLUMN(C5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ref="C5:L14" ca="1" si="0">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C5)-ROW($C$5))*32+COLUMN(C5)-COLUMN($C$5),,,"Input data"))</f>
         <v>00AE</v>
       </c>
       <c r="D5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D5)-ROW($C$5))*32+COLUMN(D5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>499A</v>
       </c>
       <c r="E5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E5)-ROW($C$5))*32+COLUMN(E5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0000</v>
       </c>
       <c r="F5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F5)-ROW($C$5))*32+COLUMN(F5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>2061</v>
       </c>
       <c r="G5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G5)-ROW($C$5))*32+COLUMN(G5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0005</v>
       </c>
       <c r="H5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H5)-ROW($C$5))*32+COLUMN(H5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0320</v>
       </c>
       <c r="I5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I5)-ROW($C$5))*32+COLUMN(I5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>03E0</v>
       </c>
       <c r="J5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J5)-ROW($C$5))*32+COLUMN(J5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1710</v>
       </c>
       <c r="K5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K5)-ROW($C$5))*32+COLUMN(K5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>A224</v>
       </c>
       <c r="L5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L5)-ROW($C$5))*32+COLUMN(L5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0185</v>
       </c>
       <c r="M5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M5)-ROW($C$5))*32+COLUMN(M5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ref="M5:V14" ca="1" si="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M5)-ROW($C$5))*32+COLUMN(M5)-COLUMN($C$5),,,"Input data"))</f>
         <v>0499</v>
       </c>
       <c r="N5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N5)-ROW($C$5))*32+COLUMN(N5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0000</v>
       </c>
       <c r="O5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O5)-ROW($C$5))*32+COLUMN(O5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1901</v>
       </c>
       <c r="P5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P5)-ROW($C$5))*32+COLUMN(P5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0000</v>
       </c>
       <c r="Q5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q5)-ROW($C$5))*32+COLUMN(Q5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0000</v>
       </c>
       <c r="R5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R5)-ROW($C$5))*32+COLUMN(R5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>B533</v>
       </c>
       <c r="S5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S5)-ROW($C$5))*32+COLUMN(S5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>4210</v>
       </c>
       <c r="T5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T5)-ROW($C$5))*32+COLUMN(T5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FFC2</v>
       </c>
       <c r="U5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U5)-ROW($C$5))*32+COLUMN(U5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0202</v>
       </c>
       <c r="V5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V5)-ROW($C$5))*32+COLUMN(V5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0202</v>
       </c>
       <c r="W5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W5)-ROW($C$5))*32+COLUMN(W5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ref="W5:AH14" ca="1" si="2">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W5)-ROW($C$5))*32+COLUMN(W5)-COLUMN($C$5),,,"Input data"))</f>
         <v>F202</v>
       </c>
       <c r="X5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X5)-ROW($C$5))*32+COLUMN(X5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F1F2</v>
       </c>
       <c r="Y5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y5)-ROW($C$5))*32+COLUMN(Y5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>D1E1</v>
       </c>
       <c r="Z5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z5)-ROW($C$5))*32+COLUMN(Z5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>AFC0</v>
       </c>
       <c r="AA5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA5)-ROW($C$5))*32+COLUMN(AA5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FF00</v>
       </c>
       <c r="AB5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB5)-ROW($C$5))*32+COLUMN(AB5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F002</v>
       </c>
       <c r="AC5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC5)-ROW($C$5))*32+COLUMN(AC5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F103</v>
       </c>
       <c r="AD5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD5)-ROW($C$5))*32+COLUMN(AD5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>E103</v>
       </c>
       <c r="AE5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE5)-ROW($C$5))*32+COLUMN(AE5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>E1F5</v>
       </c>
       <c r="AF5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF5)-ROW($C$5))*32+COLUMN(AF5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>D1E4</v>
       </c>
       <c r="AG5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG5)-ROW($C$5))*32+COLUMN(AG5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>C1D5</v>
       </c>
       <c r="AH5" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH5)-ROW($C$5))*32+COLUMN(AH5)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>91C2</v>
       </c>
     </row>
@@ -22594,131 +22743,131 @@
         <v>643</v>
       </c>
       <c r="C6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C6)-ROW($C$5))*32+COLUMN(C6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>8895</v>
       </c>
       <c r="D6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D6)-ROW($C$5))*32+COLUMN(D6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>30D9</v>
       </c>
       <c r="E6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E6)-ROW($C$5))*32+COLUMN(E6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>EDCB</v>
       </c>
       <c r="F6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F6)-ROW($C$5))*32+COLUMN(F6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>110F</v>
       </c>
       <c r="G6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G6)-ROW($C$5))*32+COLUMN(G6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3322</v>
       </c>
       <c r="H6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H6)-ROW($C$5))*32+COLUMN(H6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>2233</v>
       </c>
       <c r="I6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I6)-ROW($C$5))*32+COLUMN(I6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0011</v>
       </c>
       <c r="J6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J6)-ROW($C$5))*32+COLUMN(J6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>CCEE</v>
       </c>
       <c r="K6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K6)-ROW($C$5))*32+COLUMN(K6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FFED</v>
       </c>
       <c r="L6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L6)-ROW($C$5))*32+COLUMN(L6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1100</v>
       </c>
       <c r="M6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M6)-ROW($C$5))*32+COLUMN(M6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>2222</v>
       </c>
       <c r="N6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N6)-ROW($C$5))*32+COLUMN(N6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>3333</v>
       </c>
       <c r="O6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O6)-ROW($C$5))*32+COLUMN(O6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>2233</v>
       </c>
       <c r="P6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P6)-ROW($C$5))*32+COLUMN(P6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0022</v>
       </c>
       <c r="Q6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q6)-ROW($C$5))*32+COLUMN(Q6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>DEF0</v>
       </c>
       <c r="R6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R6)-ROW($C$5))*32+COLUMN(R6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>9ACC</v>
       </c>
       <c r="S6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S6)-ROW($C$5))*32+COLUMN(S6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>15CC</v>
       </c>
       <c r="T6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T6)-ROW($C$5))*32+COLUMN(T6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>2FA4</v>
       </c>
       <c r="U6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U6)-ROW($C$5))*32+COLUMN(U6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>2555</v>
       </c>
       <c r="V6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V6)-ROW($C$5))*32+COLUMN(V6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>9C78</v>
       </c>
       <c r="W6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W6)-ROW($C$5))*32+COLUMN(W6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>7666</v>
       </c>
       <c r="X6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X6)-ROW($C$5))*32+COLUMN(X6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>01C8</v>
       </c>
       <c r="Y6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y6)-ROW($C$5))*32+COLUMN(Y6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>3B38</v>
       </c>
       <c r="Z6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z6)-ROW($C$5))*32+COLUMN(Z6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>3534</v>
       </c>
       <c r="AA6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA6)-ROW($C$5))*32+COLUMN(AA6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>2452</v>
       </c>
       <c r="AB6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB6)-ROW($C$5))*32+COLUMN(AB6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0463</v>
       </c>
       <c r="AC6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC6)-ROW($C$5))*32+COLUMN(AC6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>13BB</v>
       </c>
       <c r="AD6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD6)-ROW($C$5))*32+COLUMN(AD6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0623</v>
       </c>
       <c r="AE6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE6)-ROW($C$5))*32+COLUMN(AE6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>EC00</v>
       </c>
       <c r="AF6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF6)-ROW($C$5))*32+COLUMN(AF6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>9797</v>
       </c>
       <c r="AG6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG6)-ROW($C$5))*32+COLUMN(AG6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>9797</v>
       </c>
       <c r="AH6" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH6)-ROW($C$5))*32+COLUMN(AH6)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>2AFB</v>
       </c>
       <c r="AI6" s="3"/>
@@ -22729,131 +22878,131 @@
         <v>644</v>
       </c>
       <c r="C7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C7)-ROW($C$5))*32+COLUMN(C7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>00AE</v>
       </c>
       <c r="D7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D7)-ROW($C$5))*32+COLUMN(D7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FBE0</v>
       </c>
       <c r="E7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E7)-ROW($C$5))*32+COLUMN(E7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1B70</v>
       </c>
       <c r="F7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F7)-ROW($C$5))*32+COLUMN(F7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>F3BE</v>
       </c>
       <c r="G7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G7)-ROW($C$5))*32+COLUMN(G7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>000E</v>
       </c>
       <c r="H7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H7)-ROW($C$5))*32+COLUMN(H7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>F86E</v>
       </c>
       <c r="I7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I7)-ROW($C$5))*32+COLUMN(I7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1B7E</v>
       </c>
       <c r="J7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J7)-ROW($C$5))*32+COLUMN(J7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>F3CE</v>
       </c>
       <c r="K7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K7)-ROW($C$5))*32+COLUMN(K7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FFCE</v>
       </c>
       <c r="L7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L7)-ROW($C$5))*32+COLUMN(L7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>F41E</v>
       </c>
       <c r="M7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M7)-ROW($C$5))*32+COLUMN(M7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>102E</v>
       </c>
       <c r="N7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N7)-ROW($C$5))*32+COLUMN(N7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>EC0E</v>
       </c>
       <c r="O7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O7)-ROW($C$5))*32+COLUMN(O7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FFDE</v>
       </c>
       <c r="P7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P7)-ROW($C$5))*32+COLUMN(P7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>EC3E</v>
       </c>
       <c r="Q7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q7)-ROW($C$5))*32+COLUMN(Q7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>139E</v>
       </c>
       <c r="R7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R7)-ROW($C$5))*32+COLUMN(R7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>EF9E</v>
       </c>
       <c r="S7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S7)-ROW($C$5))*32+COLUMN(S7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FB9E</v>
       </c>
       <c r="T7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T7)-ROW($C$5))*32+COLUMN(T7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F77E</v>
       </c>
       <c r="U7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U7)-ROW($C$5))*32+COLUMN(U7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>13E0</v>
       </c>
       <c r="V7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V7)-ROW($C$5))*32+COLUMN(V7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>E7EE</v>
       </c>
       <c r="W7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W7)-ROW($C$5))*32+COLUMN(W7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F7AE</v>
       </c>
       <c r="X7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X7)-ROW($C$5))*32+COLUMN(X7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F750</v>
       </c>
       <c r="Y7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y7)-ROW($C$5))*32+COLUMN(Y7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0C30</v>
       </c>
       <c r="Z7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z7)-ROW($C$5))*32+COLUMN(Z7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>EBEE</v>
       </c>
       <c r="AA7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA7)-ROW($C$5))*32+COLUMN(AA7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F730</v>
       </c>
       <c r="AB7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB7)-ROW($C$5))*32+COLUMN(AB7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F010</v>
       </c>
       <c r="AC7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC7)-ROW($C$5))*32+COLUMN(AC7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0B50</v>
       </c>
       <c r="AD7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD7)-ROW($C$5))*32+COLUMN(AD7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>E430</v>
       </c>
       <c r="AE7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE7)-ROW($C$5))*32+COLUMN(AE7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F420</v>
       </c>
       <c r="AF7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF7)-ROW($C$5))*32+COLUMN(AF7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F370</v>
       </c>
       <c r="AG7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG7)-ROW($C$5))*32+COLUMN(AG7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>07C0</v>
       </c>
       <c r="AH7" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH7)-ROW($C$5))*32+COLUMN(AH7)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>E450</v>
       </c>
     </row>
@@ -22863,131 +23012,131 @@
         <v>645</v>
       </c>
       <c r="C8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C8)-ROW($C$5))*32+COLUMN(C8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0470</v>
       </c>
       <c r="D8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D8)-ROW($C$5))*32+COLUMN(D8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FBCE</v>
       </c>
       <c r="E8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E8)-ROW($C$5))*32+COLUMN(E8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FF5C</v>
       </c>
       <c r="F8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F8)-ROW($C$5))*32+COLUMN(F8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0F90</v>
       </c>
       <c r="G8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G8)-ROW($C$5))*32+COLUMN(G8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>07D0</v>
       </c>
       <c r="H8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H8)-ROW($C$5))*32+COLUMN(H8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FC3E</v>
       </c>
       <c r="I8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I8)-ROW($C$5))*32+COLUMN(I8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FF6C</v>
       </c>
       <c r="J8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J8)-ROW($C$5))*32+COLUMN(J8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0F90</v>
       </c>
       <c r="K8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K8)-ROW($C$5))*32+COLUMN(K8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>03A0</v>
       </c>
       <c r="L8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L8)-ROW($C$5))*32+COLUMN(L8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FC0E</v>
       </c>
       <c r="M8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M8)-ROW($C$5))*32+COLUMN(M8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F40C</v>
       </c>
       <c r="N8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N8)-ROW($C$5))*32+COLUMN(N8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0BF0</v>
       </c>
       <c r="O8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O8)-ROW($C$5))*32+COLUMN(O8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>03A0</v>
       </c>
       <c r="P8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P8)-ROW($C$5))*32+COLUMN(P8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F41E</v>
       </c>
       <c r="Q8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q8)-ROW($C$5))*32+COLUMN(Q8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F78C</v>
       </c>
       <c r="R8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R8)-ROW($C$5))*32+COLUMN(R8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0B70</v>
       </c>
       <c r="S8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S8)-ROW($C$5))*32+COLUMN(S8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FF72</v>
       </c>
       <c r="T8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T8)-ROW($C$5))*32+COLUMN(T8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FF6E</v>
       </c>
       <c r="U8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U8)-ROW($C$5))*32+COLUMN(U8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F7DE</v>
       </c>
       <c r="V8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V8)-ROW($C$5))*32+COLUMN(V8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>07C0</v>
       </c>
       <c r="W8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W8)-ROW($C$5))*32+COLUMN(W8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FFA2</v>
       </c>
       <c r="X8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X8)-ROW($C$5))*32+COLUMN(X8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0330</v>
       </c>
       <c r="Y8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y8)-ROW($C$5))*32+COLUMN(Y8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F42E</v>
       </c>
       <c r="Z8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z8)-ROW($C$5))*32+COLUMN(Z8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0BC0</v>
       </c>
       <c r="AA8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA8)-ROW($C$5))*32+COLUMN(AA8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FF22</v>
       </c>
       <c r="AB8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB8)-ROW($C$5))*32+COLUMN(AB8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FC00</v>
       </c>
       <c r="AC8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC8)-ROW($C$5))*32+COLUMN(AC8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F75E</v>
       </c>
       <c r="AD8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD8)-ROW($C$5))*32+COLUMN(AD8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0410</v>
       </c>
       <c r="AE8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE8)-ROW($C$5))*32+COLUMN(AE8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0022</v>
       </c>
       <c r="AF8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF8)-ROW($C$5))*32+COLUMN(AF8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0350</v>
       </c>
       <c r="AG8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG8)-ROW($C$5))*32+COLUMN(AG8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F3A0</v>
       </c>
       <c r="AH8" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH8)-ROW($C$5))*32+COLUMN(AH8)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0832</v>
       </c>
     </row>
@@ -22997,131 +23146,131 @@
         <v>646</v>
       </c>
       <c r="C9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C9)-ROW($C$5))*32+COLUMN(C9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>04DE</v>
       </c>
       <c r="D9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D9)-ROW($C$5))*32+COLUMN(D9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FBF0</v>
       </c>
       <c r="E9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E9)-ROW($C$5))*32+COLUMN(E9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1BCE</v>
       </c>
       <c r="F9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F9)-ROW($C$5))*32+COLUMN(F9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>F00E</v>
       </c>
       <c r="G9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G9)-ROW($C$5))*32+COLUMN(G9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FC5E</v>
       </c>
       <c r="H9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H9)-ROW($C$5))*32+COLUMN(H9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FC80</v>
       </c>
       <c r="I9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I9)-ROW($C$5))*32+COLUMN(I9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1BF0</v>
       </c>
       <c r="J9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J9)-ROW($C$5))*32+COLUMN(J9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>F02E</v>
       </c>
       <c r="K9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K9)-ROW($C$5))*32+COLUMN(K9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0002</v>
       </c>
       <c r="L9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L9)-ROW($C$5))*32+COLUMN(L9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>F81E</v>
       </c>
       <c r="M9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M9)-ROW($C$5))*32+COLUMN(M9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>142E</v>
       </c>
       <c r="N9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N9)-ROW($C$5))*32+COLUMN(N9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>EC9E</v>
       </c>
       <c r="O9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O9)-ROW($C$5))*32+COLUMN(O9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>07DE</v>
       </c>
       <c r="P9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P9)-ROW($C$5))*32+COLUMN(P9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F09E</v>
       </c>
       <c r="Q9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q9)-ROW($C$5))*32+COLUMN(Q9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>17CE</v>
       </c>
       <c r="R9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R9)-ROW($C$5))*32+COLUMN(R9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F3AE</v>
       </c>
       <c r="S9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S9)-ROW($C$5))*32+COLUMN(S9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FFC0</v>
       </c>
       <c r="T9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T9)-ROW($C$5))*32+COLUMN(T9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FBB0</v>
       </c>
       <c r="U9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U9)-ROW($C$5))*32+COLUMN(U9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1080</v>
       </c>
       <c r="V9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V9)-ROW($C$5))*32+COLUMN(V9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>EBFE</v>
       </c>
       <c r="W9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W9)-ROW($C$5))*32+COLUMN(W9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FFE0</v>
       </c>
       <c r="X9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X9)-ROW($C$5))*32+COLUMN(X9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FF90</v>
       </c>
       <c r="Y9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y9)-ROW($C$5))*32+COLUMN(Y9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>1460</v>
       </c>
       <c r="Z9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z9)-ROW($C$5))*32+COLUMN(Z9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>E4AE</v>
       </c>
       <c r="AA9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA9)-ROW($C$5))*32+COLUMN(AA9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FBC0</v>
       </c>
       <c r="AB9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB9)-ROW($C$5))*32+COLUMN(AB9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F840</v>
       </c>
       <c r="AC9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC9)-ROW($C$5))*32+COLUMN(AC9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0FE0</v>
       </c>
       <c r="AD9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD9)-ROW($C$5))*32+COLUMN(AD9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>E860</v>
       </c>
       <c r="AE9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE9)-ROW($C$5))*32+COLUMN(AE9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F8C0</v>
       </c>
       <c r="AF9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF9)-ROW($C$5))*32+COLUMN(AF9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F400</v>
       </c>
       <c r="AG9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG9)-ROW($C$5))*32+COLUMN(AG9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0842</v>
       </c>
       <c r="AH9" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH9)-ROW($C$5))*32+COLUMN(AH9)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>E4B0</v>
       </c>
     </row>
@@ -23131,131 +23280,131 @@
         <v>647</v>
       </c>
       <c r="C10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C10)-ROW($C$5))*32+COLUMN(C10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0890</v>
       </c>
       <c r="D10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D10)-ROW($C$5))*32+COLUMN(D10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>03BE</v>
       </c>
       <c r="E10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E10)-ROW($C$5))*32+COLUMN(E10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FF9C</v>
       </c>
       <c r="F10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F10)-ROW($C$5))*32+COLUMN(F10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0FD0</v>
       </c>
       <c r="G10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G10)-ROW($C$5))*32+COLUMN(G10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0020</v>
       </c>
       <c r="H10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H10)-ROW($C$5))*32+COLUMN(H10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0450</v>
       </c>
       <c r="I10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I10)-ROW($C$5))*32+COLUMN(I10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FFCC</v>
       </c>
       <c r="J10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J10)-ROW($C$5))*32+COLUMN(J10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0FE0</v>
       </c>
       <c r="K10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K10)-ROW($C$5))*32+COLUMN(K10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>07D0</v>
       </c>
       <c r="L10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L10)-ROW($C$5))*32+COLUMN(L10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>03FE</v>
       </c>
       <c r="M10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M10)-ROW($C$5))*32+COLUMN(M10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FBEE</v>
       </c>
       <c r="N10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N10)-ROW($C$5))*32+COLUMN(N10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0C60</v>
       </c>
       <c r="O10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O10)-ROW($C$5))*32+COLUMN(O10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0B80</v>
       </c>
       <c r="P10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P10)-ROW($C$5))*32+COLUMN(P10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F86E</v>
       </c>
       <c r="Q10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q10)-ROW($C$5))*32+COLUMN(Q10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FB8E</v>
       </c>
       <c r="R10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R10)-ROW($C$5))*32+COLUMN(R10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1370</v>
       </c>
       <c r="S10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S10)-ROW($C$5))*32+COLUMN(S10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0782</v>
       </c>
       <c r="T10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T10)-ROW($C$5))*32+COLUMN(T10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>038E</v>
       </c>
       <c r="U10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U10)-ROW($C$5))*32+COLUMN(U10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F85E</v>
       </c>
       <c r="V10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V10)-ROW($C$5))*32+COLUMN(V10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0FC2</v>
       </c>
       <c r="W10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W10)-ROW($C$5))*32+COLUMN(W10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>07C2</v>
       </c>
       <c r="X10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X10)-ROW($C$5))*32+COLUMN(X10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>037E</v>
       </c>
       <c r="Y10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y10)-ROW($C$5))*32+COLUMN(Y10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F84E</v>
       </c>
       <c r="Z10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z10)-ROW($C$5))*32+COLUMN(Z10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0880</v>
       </c>
       <c r="AA10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA10)-ROW($C$5))*32+COLUMN(AA10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0392</v>
       </c>
       <c r="AB10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB10)-ROW($C$5))*32+COLUMN(AB10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0420</v>
       </c>
       <c r="AC10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC10)-ROW($C$5))*32+COLUMN(AC10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F7CE</v>
       </c>
       <c r="AD10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD10)-ROW($C$5))*32+COLUMN(AD10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0C42</v>
       </c>
       <c r="AE10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE10)-ROW($C$5))*32+COLUMN(AE10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FCB2</v>
       </c>
       <c r="AF10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF10)-ROW($C$5))*32+COLUMN(AF10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FFE0</v>
       </c>
       <c r="AG10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG10)-ROW($C$5))*32+COLUMN(AG10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F020</v>
       </c>
       <c r="AH10" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH10)-ROW($C$5))*32+COLUMN(AH10)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0490</v>
       </c>
     </row>
@@ -23265,131 +23414,131 @@
         <v>648</v>
       </c>
       <c r="C11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C11)-ROW($C$5))*32+COLUMN(C11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>107E</v>
       </c>
       <c r="D11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D11)-ROW($C$5))*32+COLUMN(D11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>03D0</v>
       </c>
       <c r="E11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E11)-ROW($C$5))*32+COLUMN(E11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1F90</v>
       </c>
       <c r="F11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F11)-ROW($C$5))*32+COLUMN(F11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FBCE</v>
       </c>
       <c r="G11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G11)-ROW($C$5))*32+COLUMN(G11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>089E</v>
       </c>
       <c r="H11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H11)-ROW($C$5))*32+COLUMN(H11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0080</v>
       </c>
       <c r="I11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I11)-ROW($C$5))*32+COLUMN(I11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1820</v>
       </c>
       <c r="J11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J11)-ROW($C$5))*32+COLUMN(J11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>F40E</v>
       </c>
       <c r="K11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K11)-ROW($C$5))*32+COLUMN(K11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0800</v>
       </c>
       <c r="L11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L11)-ROW($C$5))*32+COLUMN(L11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FC30</v>
       </c>
       <c r="M11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M11)-ROW($C$5))*32+COLUMN(M11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>141E</v>
       </c>
       <c r="N11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N11)-ROW($C$5))*32+COLUMN(N11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F06E</v>
       </c>
       <c r="O11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O11)-ROW($C$5))*32+COLUMN(O11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0400</v>
       </c>
       <c r="P11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P11)-ROW($C$5))*32+COLUMN(P11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FFA0</v>
       </c>
       <c r="Q11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q11)-ROW($C$5))*32+COLUMN(Q11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>17CE</v>
       </c>
       <c r="R11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R11)-ROW($C$5))*32+COLUMN(R11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F7B0</v>
       </c>
       <c r="S11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S11)-ROW($C$5))*32+COLUMN(S11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>07D0</v>
       </c>
       <c r="T11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T11)-ROW($C$5))*32+COLUMN(T11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FFB0</v>
       </c>
       <c r="U11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U11)-ROW($C$5))*32+COLUMN(U11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1830</v>
       </c>
       <c r="V11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V11)-ROW($C$5))*32+COLUMN(V11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F3FE</v>
       </c>
       <c r="W11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W11)-ROW($C$5))*32+COLUMN(W11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0002</v>
       </c>
       <c r="X11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X11)-ROW($C$5))*32+COLUMN(X11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FFE0</v>
       </c>
       <c r="Y11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y11)-ROW($C$5))*32+COLUMN(Y11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>14D0</v>
       </c>
       <c r="Z11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z11)-ROW($C$5))*32+COLUMN(Z11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>ECB0</v>
       </c>
       <c r="AA11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA11)-ROW($C$5))*32+COLUMN(AA11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FBE2</v>
       </c>
       <c r="AB11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB11)-ROW($C$5))*32+COLUMN(AB11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FCB0</v>
       </c>
       <c r="AC11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC11)-ROW($C$5))*32+COLUMN(AC11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>13B0</v>
       </c>
       <c r="AD11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD11)-ROW($C$5))*32+COLUMN(AD11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>ECA0</v>
       </c>
       <c r="AE11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE11)-ROW($C$5))*32+COLUMN(AE11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F8DE</v>
       </c>
       <c r="AF11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF11)-ROW($C$5))*32+COLUMN(AF11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F432</v>
       </c>
       <c r="AG11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG11)-ROW($C$5))*32+COLUMN(AG11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0832</v>
       </c>
       <c r="AH11" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH11)-ROW($C$5))*32+COLUMN(AH11)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>E8D0</v>
       </c>
     </row>
@@ -23399,131 +23548,131 @@
         <v>649</v>
       </c>
       <c r="C12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C12)-ROW($C$5))*32+COLUMN(C12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1420</v>
       </c>
       <c r="D12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D12)-ROW($C$5))*32+COLUMN(D12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FF8E</v>
       </c>
       <c r="E12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E12)-ROW($C$5))*32+COLUMN(E12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FF6E</v>
       </c>
       <c r="F12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F12)-ROW($C$5))*32+COLUMN(F12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1380</v>
       </c>
       <c r="G12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G12)-ROW($C$5))*32+COLUMN(G12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0840</v>
       </c>
       <c r="H12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H12)-ROW($C$5))*32+COLUMN(H12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>005E</v>
       </c>
       <c r="I12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I12)-ROW($C$5))*32+COLUMN(I12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FBEC</v>
       </c>
       <c r="J12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J12)-ROW($C$5))*32+COLUMN(J12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0FB0</v>
       </c>
       <c r="K12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K12)-ROW($C$5))*32+COLUMN(K12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0BB2</v>
       </c>
       <c r="L12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L12)-ROW($C$5))*32+COLUMN(L12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FFFE</v>
       </c>
       <c r="M12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M12)-ROW($C$5))*32+COLUMN(M12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FBDE</v>
       </c>
       <c r="N12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N12)-ROW($C$5))*32+COLUMN(N12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0820</v>
       </c>
       <c r="O12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O12)-ROW($C$5))*32+COLUMN(O12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0BC0</v>
       </c>
       <c r="P12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P12)-ROW($C$5))*32+COLUMN(P12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0360</v>
       </c>
       <c r="Q12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q12)-ROW($C$5))*32+COLUMN(Q12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FB8C</v>
       </c>
       <c r="R12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R12)-ROW($C$5))*32+COLUMN(R12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0F70</v>
       </c>
       <c r="S12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S12)-ROW($C$5))*32+COLUMN(S12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0794</v>
       </c>
       <c r="T12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T12)-ROW($C$5))*32+COLUMN(T12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>036E</v>
       </c>
       <c r="U12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U12)-ROW($C$5))*32+COLUMN(U12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FBFE</v>
       </c>
       <c r="V12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V12)-ROW($C$5))*32+COLUMN(V12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0FA0</v>
       </c>
       <c r="W12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W12)-ROW($C$5))*32+COLUMN(W12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0BC4</v>
       </c>
       <c r="X12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X12)-ROW($C$5))*32+COLUMN(X12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0390</v>
       </c>
       <c r="Y12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y12)-ROW($C$5))*32+COLUMN(Y12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F89E</v>
       </c>
       <c r="Z12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z12)-ROW($C$5))*32+COLUMN(Z12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0C72</v>
       </c>
       <c r="AA12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA12)-ROW($C$5))*32+COLUMN(AA12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FFB2</v>
       </c>
       <c r="AB12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB12)-ROW($C$5))*32+COLUMN(AB12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FC70</v>
       </c>
       <c r="AC12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC12)-ROW($C$5))*32+COLUMN(AC12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FB7E</v>
       </c>
       <c r="AD12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD12)-ROW($C$5))*32+COLUMN(AD12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0470</v>
       </c>
       <c r="AE12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE12)-ROW($C$5))*32+COLUMN(AE12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FCB0</v>
       </c>
       <c r="AF12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF12)-ROW($C$5))*32+COLUMN(AF12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FFF0</v>
       </c>
       <c r="AG12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG12)-ROW($C$5))*32+COLUMN(AG12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F3F0</v>
       </c>
       <c r="AH12" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH12)-ROW($C$5))*32+COLUMN(AH12)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>04A0</v>
       </c>
     </row>
@@ -23533,131 +23682,131 @@
         <v>650</v>
       </c>
       <c r="C13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C13)-ROW($C$5))*32+COLUMN(C13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>049E</v>
       </c>
       <c r="D13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D13)-ROW($C$5))*32+COLUMN(D13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>03B0</v>
       </c>
       <c r="E13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E13)-ROW($C$5))*32+COLUMN(E13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1F90</v>
       </c>
       <c r="F13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F13)-ROW($C$5))*32+COLUMN(F13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>F7D0</v>
       </c>
       <c r="G13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G13)-ROW($C$5))*32+COLUMN(G13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>042E</v>
       </c>
       <c r="H13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H13)-ROW($C$5))*32+COLUMN(H13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0070</v>
       </c>
       <c r="I13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I13)-ROW($C$5))*32+COLUMN(I13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1F70</v>
       </c>
       <c r="J13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J13)-ROW($C$5))*32+COLUMN(J13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FBBE</v>
       </c>
       <c r="K13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K13)-ROW($C$5))*32+COLUMN(K13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0F00</v>
       </c>
       <c r="L13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L13)-ROW($C$5))*32+COLUMN(L13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>03B0</v>
       </c>
       <c r="M13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M13)-ROW($C$5))*32+COLUMN(M13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>142E</v>
       </c>
       <c r="N13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N13)-ROW($C$5))*32+COLUMN(N13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F01E</v>
       </c>
       <c r="O13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O13)-ROW($C$5))*32+COLUMN(O13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>07B0</v>
       </c>
       <c r="P13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P13)-ROW($C$5))*32+COLUMN(P13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FFB0</v>
       </c>
       <c r="Q13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q13)-ROW($C$5))*32+COLUMN(Q13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1B60</v>
       </c>
       <c r="R13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R13)-ROW($C$5))*32+COLUMN(R13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F37E</v>
       </c>
       <c r="S13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S13)-ROW($C$5))*32+COLUMN(S13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FBD0</v>
       </c>
       <c r="T13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T13)-ROW($C$5))*32+COLUMN(T13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FF90</v>
       </c>
       <c r="U13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U13)-ROW($C$5))*32+COLUMN(U13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>1410</v>
       </c>
       <c r="V13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V13)-ROW($C$5))*32+COLUMN(V13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F3C0</v>
       </c>
       <c r="W13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W13)-ROW($C$5))*32+COLUMN(W13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FC00</v>
       </c>
       <c r="X13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X13)-ROW($C$5))*32+COLUMN(X13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0370</v>
       </c>
       <c r="Y13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y13)-ROW($C$5))*32+COLUMN(Y13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>1482</v>
       </c>
       <c r="Z13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z13)-ROW($C$5))*32+COLUMN(Z13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F030</v>
       </c>
       <c r="AA13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA13)-ROW($C$5))*32+COLUMN(AA13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F800</v>
       </c>
       <c r="AB13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB13)-ROW($C$5))*32+COLUMN(AB13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FC50</v>
       </c>
       <c r="AC13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC13)-ROW($C$5))*32+COLUMN(AC13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>13C2</v>
       </c>
       <c r="AD13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD13)-ROW($C$5))*32+COLUMN(AD13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F050</v>
       </c>
       <c r="AE13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE13)-ROW($C$5))*32+COLUMN(AE13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0070</v>
       </c>
       <c r="AF13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF13)-ROW($C$5))*32+COLUMN(AF13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F812</v>
       </c>
       <c r="AG13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG13)-ROW($C$5))*32+COLUMN(AG13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0C02</v>
       </c>
       <c r="AH13" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH13)-ROW($C$5))*32+COLUMN(AH13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>EC80</v>
       </c>
     </row>
@@ -23667,131 +23816,131 @@
         <v>651</v>
       </c>
       <c r="C14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C14)-ROW($C$5))*32+COLUMN(C14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>00D0</v>
       </c>
       <c r="D14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D14)-ROW($C$5))*32+COLUMN(D14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FBFE</v>
       </c>
       <c r="E14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E14)-ROW($C$5))*32+COLUMN(E14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FBCC</v>
       </c>
       <c r="F14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F14)-ROW($C$5))*32+COLUMN(F14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0810</v>
       </c>
       <c r="G14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G14)-ROW($C$5))*32+COLUMN(G14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FC60</v>
       </c>
       <c r="H14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H14)-ROW($C$5))*32+COLUMN(H14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FCB0</v>
       </c>
       <c r="I14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I14)-ROW($C$5))*32+COLUMN(I14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FBCE</v>
       </c>
       <c r="J14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J14)-ROW($C$5))*32+COLUMN(J14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0FE0</v>
       </c>
       <c r="K14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K14)-ROW($C$5))*32+COLUMN(K14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0B40</v>
       </c>
       <c r="L14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L14)-ROW($C$5))*32+COLUMN(L14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="0"/>
         <v>FFFE</v>
       </c>
       <c r="M14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M14)-ROW($C$5))*32+COLUMN(M14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F05C</v>
       </c>
       <c r="N14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N14)-ROW($C$5))*32+COLUMN(N14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0840</v>
       </c>
       <c r="O14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O14)-ROW($C$5))*32+COLUMN(O14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>07D0</v>
       </c>
       <c r="P14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P14)-ROW($C$5))*32+COLUMN(P14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FFD0</v>
       </c>
       <c r="Q14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q14)-ROW($C$5))*32+COLUMN(Q14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F79E</v>
       </c>
       <c r="R14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R14)-ROW($C$5))*32+COLUMN(R14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0FB0</v>
       </c>
       <c r="S14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S14)-ROW($C$5))*32+COLUMN(S14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F802</v>
       </c>
       <c r="T14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T14)-ROW($C$5))*32+COLUMN(T14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>FFD0</v>
       </c>
       <c r="U14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U14)-ROW($C$5))*32+COLUMN(U14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>F44E</v>
       </c>
       <c r="V14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V14)-ROW($C$5))*32+COLUMN(V14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0BF0</v>
       </c>
       <c r="W14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W14)-ROW($C$5))*32+COLUMN(W14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>FC32</v>
       </c>
       <c r="X14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X14)-ROW($C$5))*32+COLUMN(X14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>07A0</v>
       </c>
       <c r="Y14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y14)-ROW($C$5))*32+COLUMN(Y14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F4BE</v>
       </c>
       <c r="Z14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z14)-ROW($C$5))*32+COLUMN(Z14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0C60</v>
       </c>
       <c r="AA14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA14)-ROW($C$5))*32+COLUMN(AA14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F822</v>
       </c>
       <c r="AB14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB14)-ROW($C$5))*32+COLUMN(AB14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0080</v>
       </c>
       <c r="AC14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC14)-ROW($C$5))*32+COLUMN(AC14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F01E</v>
       </c>
       <c r="AD14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD14)-ROW($C$5))*32+COLUMN(AD14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>0892</v>
       </c>
       <c r="AE14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE14)-ROW($C$5))*32+COLUMN(AE14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>00B4</v>
       </c>
       <c r="AF14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF14)-ROW($C$5))*32+COLUMN(AF14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F850</v>
       </c>
       <c r="AG14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG14)-ROW($C$5))*32+COLUMN(AG14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>F040</v>
       </c>
       <c r="AH14" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH14)-ROW($C$5))*32+COLUMN(AH14)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="2"/>
         <v>04B2</v>
       </c>
     </row>
@@ -23801,131 +23950,131 @@
         <v>652</v>
       </c>
       <c r="C15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C15)-ROW($C$5))*32+COLUMN(C15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ref="C15:L24" ca="1" si="3">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C15)-ROW($C$5))*32+COLUMN(C15)-COLUMN($C$5),,,"Input data"))</f>
         <v>085E</v>
       </c>
       <c r="D15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D15)-ROW($C$5))*32+COLUMN(D15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0782</v>
       </c>
       <c r="E15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E15)-ROW($C$5))*32+COLUMN(E15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1F70</v>
       </c>
       <c r="F15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F15)-ROW($C$5))*32+COLUMN(F15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FBEE</v>
       </c>
       <c r="G15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G15)-ROW($C$5))*32+COLUMN(G15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>001E</v>
       </c>
       <c r="H15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H15)-ROW($C$5))*32+COLUMN(H15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0420</v>
       </c>
       <c r="I15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I15)-ROW($C$5))*32+COLUMN(I15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1F80</v>
       </c>
       <c r="J15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J15)-ROW($C$5))*32+COLUMN(J15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FBB0</v>
       </c>
       <c r="K15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K15)-ROW($C$5))*32+COLUMN(K15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>03B0</v>
       </c>
       <c r="L15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L15)-ROW($C$5))*32+COLUMN(L15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0390</v>
       </c>
       <c r="M15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M15)-ROW($C$5))*32+COLUMN(M15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ref="M15:V24" ca="1" si="4">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M15)-ROW($C$5))*32+COLUMN(M15)-COLUMN($C$5),,,"Input data"))</f>
         <v>17F0</v>
       </c>
       <c r="N15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N15)-ROW($C$5))*32+COLUMN(N15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F04E</v>
       </c>
       <c r="O15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O15)-ROW($C$5))*32+COLUMN(O15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0770</v>
       </c>
       <c r="P15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P15)-ROW($C$5))*32+COLUMN(P15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FFE0</v>
       </c>
       <c r="Q15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q15)-ROW($C$5))*32+COLUMN(Q15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1B40</v>
       </c>
       <c r="R15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R15)-ROW($C$5))*32+COLUMN(R15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F76E</v>
       </c>
       <c r="S15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S15)-ROW($C$5))*32+COLUMN(S15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FFC0</v>
       </c>
       <c r="T15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T15)-ROW($C$5))*32+COLUMN(T15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FFB0</v>
       </c>
       <c r="U15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U15)-ROW($C$5))*32+COLUMN(U15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>17E0</v>
       </c>
       <c r="V15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V15)-ROW($C$5))*32+COLUMN(V15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>EC1E</v>
       </c>
       <c r="W15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W15)-ROW($C$5))*32+COLUMN(W15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ref="W15:AH24" ca="1" si="5">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W15)-ROW($C$5))*32+COLUMN(W15)-COLUMN($C$5),,,"Input data"))</f>
         <v>03A0</v>
       </c>
       <c r="X15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X15)-ROW($C$5))*32+COLUMN(X15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>03A0</v>
       </c>
       <c r="Y15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y15)-ROW($C$5))*32+COLUMN(Y15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>10C0</v>
       </c>
       <c r="Z15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z15)-ROW($C$5))*32+COLUMN(Z15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>EC60</v>
       </c>
       <c r="AA15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA15)-ROW($C$5))*32+COLUMN(AA15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FBC2</v>
       </c>
       <c r="AB15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB15)-ROW($C$5))*32+COLUMN(AB15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FC80</v>
       </c>
       <c r="AC15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC15)-ROW($C$5))*32+COLUMN(AC15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0C00</v>
       </c>
       <c r="AD15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD15)-ROW($C$5))*32+COLUMN(AD15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>EC60</v>
       </c>
       <c r="AE15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE15)-ROW($C$5))*32+COLUMN(AE15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0050</v>
       </c>
       <c r="AF15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF15)-ROW($C$5))*32+COLUMN(AF15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F800</v>
       </c>
       <c r="AG15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG15)-ROW($C$5))*32+COLUMN(AG15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0802</v>
       </c>
       <c r="AH15" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH15)-ROW($C$5))*32+COLUMN(AH15)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>EC90</v>
       </c>
     </row>
@@ -23935,131 +24084,131 @@
         <v>653</v>
       </c>
       <c r="C16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C16)-ROW($C$5))*32+COLUMN(C16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0080</v>
       </c>
       <c r="D16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D16)-ROW($C$5))*32+COLUMN(D16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F7B0</v>
       </c>
       <c r="E16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E16)-ROW($C$5))*32+COLUMN(E16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F7AE</v>
       </c>
       <c r="F16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F16)-ROW($C$5))*32+COLUMN(F16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0410</v>
       </c>
       <c r="G16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G16)-ROW($C$5))*32+COLUMN(G16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FC32</v>
       </c>
       <c r="H16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H16)-ROW($C$5))*32+COLUMN(H16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FC50</v>
       </c>
       <c r="I16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I16)-ROW($C$5))*32+COLUMN(I16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F7BE</v>
       </c>
       <c r="J16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J16)-ROW($C$5))*32+COLUMN(J16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>07F0</v>
       </c>
       <c r="K16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K16)-ROW($C$5))*32+COLUMN(K16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FFD2</v>
       </c>
       <c r="L16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L16)-ROW($C$5))*32+COLUMN(L16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FBC0</v>
       </c>
       <c r="M16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M16)-ROW($C$5))*32+COLUMN(M16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F02E</v>
       </c>
       <c r="N16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N16)-ROW($C$5))*32+COLUMN(N16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0460</v>
       </c>
       <c r="O16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O16)-ROW($C$5))*32+COLUMN(O16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0382</v>
       </c>
       <c r="P16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P16)-ROW($C$5))*32+COLUMN(P16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F410</v>
       </c>
       <c r="Q16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q16)-ROW($C$5))*32+COLUMN(Q16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F36E</v>
       </c>
       <c r="R16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R16)-ROW($C$5))*32+COLUMN(R16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0BA0</v>
       </c>
       <c r="S16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S16)-ROW($C$5))*32+COLUMN(S16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FBF2</v>
       </c>
       <c r="T16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T16)-ROW($C$5))*32+COLUMN(T16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FBC0</v>
       </c>
       <c r="U16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U16)-ROW($C$5))*32+COLUMN(U16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F01C</v>
       </c>
       <c r="V16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V16)-ROW($C$5))*32+COLUMN(V16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0440</v>
       </c>
       <c r="W16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W16)-ROW($C$5))*32+COLUMN(W16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FFE2</v>
       </c>
       <c r="X16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X16)-ROW($C$5))*32+COLUMN(X16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FBE0</v>
       </c>
       <c r="Y16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y16)-ROW($C$5))*32+COLUMN(Y16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F0EE</v>
       </c>
       <c r="Z16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z16)-ROW($C$5))*32+COLUMN(Z16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>08A2</v>
       </c>
       <c r="AA16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA16)-ROW($C$5))*32+COLUMN(AA16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F804</v>
       </c>
       <c r="AB16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB16)-ROW($C$5))*32+COLUMN(AB16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FCB0</v>
       </c>
       <c r="AC16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC16)-ROW($C$5))*32+COLUMN(AC16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>EC3E</v>
       </c>
       <c r="AD16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD16)-ROW($C$5))*32+COLUMN(AD16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>04A2</v>
       </c>
       <c r="AE16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE16)-ROW($C$5))*32+COLUMN(AE16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0082</v>
       </c>
       <c r="AF16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF16)-ROW($C$5))*32+COLUMN(AF16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F830</v>
       </c>
       <c r="AG16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG16)-ROW($C$5))*32+COLUMN(AG16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>E830</v>
       </c>
       <c r="AH16" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH16)-ROW($C$5))*32+COLUMN(AH16)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>04B2</v>
       </c>
     </row>
@@ -24069,131 +24218,131 @@
         <v>654</v>
       </c>
       <c r="C17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C17)-ROW($C$5))*32+COLUMN(C17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>13F0</v>
       </c>
       <c r="D17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D17)-ROW($C$5))*32+COLUMN(D17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0380</v>
       </c>
       <c r="E17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E17)-ROW($C$5))*32+COLUMN(E17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1F40</v>
       </c>
       <c r="F17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F17)-ROW($C$5))*32+COLUMN(F17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FBB0</v>
       </c>
       <c r="G17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G17)-ROW($C$5))*32+COLUMN(G17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0F90</v>
       </c>
       <c r="H17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H17)-ROW($C$5))*32+COLUMN(H17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0420</v>
       </c>
       <c r="I17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I17)-ROW($C$5))*32+COLUMN(I17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>17A0</v>
       </c>
       <c r="J17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J17)-ROW($C$5))*32+COLUMN(J17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F7AE</v>
       </c>
       <c r="K17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K17)-ROW($C$5))*32+COLUMN(K17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0F40</v>
       </c>
       <c r="L17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L17)-ROW($C$5))*32+COLUMN(L17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FFE2</v>
       </c>
       <c r="M17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M17)-ROW($C$5))*32+COLUMN(M17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>13AE</v>
       </c>
       <c r="N17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N17)-ROW($C$5))*32+COLUMN(N17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F03E</v>
       </c>
       <c r="O17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O17)-ROW($C$5))*32+COLUMN(O17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0F12</v>
       </c>
       <c r="P17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P17)-ROW($C$5))*32+COLUMN(P17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FF60</v>
       </c>
       <c r="Q17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q17)-ROW($C$5))*32+COLUMN(Q17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0F50</v>
       </c>
       <c r="R17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R17)-ROW($C$5))*32+COLUMN(R17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F340</v>
       </c>
       <c r="S17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S17)-ROW($C$5))*32+COLUMN(S17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0362</v>
       </c>
       <c r="T17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T17)-ROW($C$5))*32+COLUMN(T17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FF30</v>
       </c>
       <c r="U17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U17)-ROW($C$5))*32+COLUMN(U17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1760</v>
       </c>
       <c r="V17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V17)-ROW($C$5))*32+COLUMN(V17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>EFD0</v>
       </c>
       <c r="W17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W17)-ROW($C$5))*32+COLUMN(W17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0762</v>
       </c>
       <c r="X17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X17)-ROW($C$5))*32+COLUMN(X17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0360</v>
       </c>
       <c r="Y17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y17)-ROW($C$5))*32+COLUMN(Y17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>1072</v>
       </c>
       <c r="Z17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z17)-ROW($C$5))*32+COLUMN(Z17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>EC50</v>
       </c>
       <c r="AA17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA17)-ROW($C$5))*32+COLUMN(AA17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F7B2</v>
       </c>
       <c r="AB17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB17)-ROW($C$5))*32+COLUMN(AB17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F852</v>
       </c>
       <c r="AC17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC17)-ROW($C$5))*32+COLUMN(AC17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>07B0</v>
       </c>
       <c r="AD17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD17)-ROW($C$5))*32+COLUMN(AD17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>E480</v>
       </c>
       <c r="AE17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE17)-ROW($C$5))*32+COLUMN(AE17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F820</v>
       </c>
       <c r="AF17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF17)-ROW($C$5))*32+COLUMN(AF17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F7C2</v>
       </c>
       <c r="AG17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG17)-ROW($C$5))*32+COLUMN(AG17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>03C2</v>
       </c>
       <c r="AH17" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH17)-ROW($C$5))*32+COLUMN(AH17)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>E490</v>
       </c>
     </row>
@@ -24203,131 +24352,131 @@
         <v>655</v>
       </c>
       <c r="C18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C18)-ROW($C$5))*32+COLUMN(C18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1422</v>
       </c>
       <c r="D18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D18)-ROW($C$5))*32+COLUMN(D18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>03AE</v>
       </c>
       <c r="E18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E18)-ROW($C$5))*32+COLUMN(E18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>036E</v>
       </c>
       <c r="F18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F18)-ROW($C$5))*32+COLUMN(F18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>13C2</v>
       </c>
       <c r="G18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G18)-ROW($C$5))*32+COLUMN(G18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>13B2</v>
       </c>
       <c r="H18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H18)-ROW($C$5))*32+COLUMN(H18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0440</v>
       </c>
       <c r="I18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I18)-ROW($C$5))*32+COLUMN(I18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FFCE</v>
       </c>
       <c r="J18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J18)-ROW($C$5))*32+COLUMN(J18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>13D2</v>
       </c>
       <c r="K18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K18)-ROW($C$5))*32+COLUMN(K18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1362</v>
       </c>
       <c r="L18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L18)-ROW($C$5))*32+COLUMN(L18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0002</v>
       </c>
       <c r="M18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M18)-ROW($C$5))*32+COLUMN(M18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FBDE</v>
       </c>
       <c r="N18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N18)-ROW($C$5))*32+COLUMN(N18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0C40</v>
       </c>
       <c r="O18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O18)-ROW($C$5))*32+COLUMN(O18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1732</v>
       </c>
       <c r="P18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P18)-ROW($C$5))*32+COLUMN(P18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0390</v>
       </c>
       <c r="Q18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q18)-ROW($C$5))*32+COLUMN(Q18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FF8E</v>
       </c>
       <c r="R18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R18)-ROW($C$5))*32+COLUMN(R18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1760</v>
       </c>
       <c r="S18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S18)-ROW($C$5))*32+COLUMN(S18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0B82</v>
       </c>
       <c r="T18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T18)-ROW($C$5))*32+COLUMN(T18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0750</v>
       </c>
       <c r="U18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U18)-ROW($C$5))*32+COLUMN(U18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>039E</v>
       </c>
       <c r="V18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V18)-ROW($C$5))*32+COLUMN(V18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1000</v>
       </c>
       <c r="W18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W18)-ROW($C$5))*32+COLUMN(W18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0F82</v>
       </c>
       <c r="X18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X18)-ROW($C$5))*32+COLUMN(X18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0B80</v>
       </c>
       <c r="Y18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y18)-ROW($C$5))*32+COLUMN(Y18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FCAE</v>
       </c>
       <c r="Z18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z18)-ROW($C$5))*32+COLUMN(Z18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>1080</v>
       </c>
       <c r="AA18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA18)-ROW($C$5))*32+COLUMN(AA18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0BD4</v>
       </c>
       <c r="AB18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB18)-ROW($C$5))*32+COLUMN(AB18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0470</v>
       </c>
       <c r="AC18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC18)-ROW($C$5))*32+COLUMN(AC18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FBCE</v>
       </c>
       <c r="AD18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD18)-ROW($C$5))*32+COLUMN(AD18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0C92</v>
       </c>
       <c r="AE18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE18)-ROW($C$5))*32+COLUMN(AE18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0832</v>
       </c>
       <c r="AF18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF18)-ROW($C$5))*32+COLUMN(AF18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>07E0</v>
       </c>
       <c r="AG18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG18)-ROW($C$5))*32+COLUMN(AG18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F7FE</v>
       </c>
       <c r="AH18" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH18)-ROW($C$5))*32+COLUMN(AH18)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0CA2</v>
       </c>
     </row>
@@ -24337,131 +24486,131 @@
         <v>656</v>
       </c>
       <c r="C19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C19)-ROW($C$5))*32+COLUMN(C19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0010</v>
       </c>
       <c r="D19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D19)-ROW($C$5))*32+COLUMN(D19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0380</v>
       </c>
       <c r="E19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E19)-ROW($C$5))*32+COLUMN(E19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>13D0</v>
       </c>
       <c r="F19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F19)-ROW($C$5))*32+COLUMN(F19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F7A0</v>
       </c>
       <c r="G19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G19)-ROW($C$5))*32+COLUMN(G19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FFBE</v>
       </c>
       <c r="H19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H19)-ROW($C$5))*32+COLUMN(H19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0052</v>
       </c>
       <c r="I19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I19)-ROW($C$5))*32+COLUMN(I19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1380</v>
       </c>
       <c r="J19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J19)-ROW($C$5))*32+COLUMN(J19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F770</v>
       </c>
       <c r="K19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K19)-ROW($C$5))*32+COLUMN(K19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FF70</v>
       </c>
       <c r="L19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L19)-ROW($C$5))*32+COLUMN(L19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FFA0</v>
       </c>
       <c r="M19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M19)-ROW($C$5))*32+COLUMN(M19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0FC0</v>
       </c>
       <c r="N19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N19)-ROW($C$5))*32+COLUMN(N19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F3BE</v>
       </c>
       <c r="O19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O19)-ROW($C$5))*32+COLUMN(O19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0340</v>
       </c>
       <c r="P19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P19)-ROW($C$5))*32+COLUMN(P19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FF60</v>
       </c>
       <c r="Q19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q19)-ROW($C$5))*32+COLUMN(Q19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0FC0</v>
       </c>
       <c r="R19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R19)-ROW($C$5))*32+COLUMN(R19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F370</v>
       </c>
       <c r="S19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S19)-ROW($C$5))*32+COLUMN(S19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FB30</v>
       </c>
       <c r="T19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T19)-ROW($C$5))*32+COLUMN(T19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FB80</v>
       </c>
       <c r="U19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U19)-ROW($C$5))*32+COLUMN(U19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0C10</v>
       </c>
       <c r="V19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V19)-ROW($C$5))*32+COLUMN(V19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>E40E</v>
       </c>
       <c r="W19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W19)-ROW($C$5))*32+COLUMN(W19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FBA0</v>
       </c>
       <c r="X19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X19)-ROW($C$5))*32+COLUMN(X19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FBB0</v>
       </c>
       <c r="Y19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y19)-ROW($C$5))*32+COLUMN(Y19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0C42</v>
       </c>
       <c r="Z19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z19)-ROW($C$5))*32+COLUMN(Z19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>E860</v>
       </c>
       <c r="AA19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA19)-ROW($C$5))*32+COLUMN(AA19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FB92</v>
       </c>
       <c r="AB19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB19)-ROW($C$5))*32+COLUMN(AB19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F4A2</v>
       </c>
       <c r="AC19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC19)-ROW($C$5))*32+COLUMN(AC19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0B82</v>
       </c>
       <c r="AD19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD19)-ROW($C$5))*32+COLUMN(AD19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>E850</v>
       </c>
       <c r="AE19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE19)-ROW($C$5))*32+COLUMN(AE19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F832</v>
       </c>
       <c r="AF19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF19)-ROW($C$5))*32+COLUMN(AF19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FBA2</v>
       </c>
       <c r="AG19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG19)-ROW($C$5))*32+COLUMN(AG19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0002</v>
       </c>
       <c r="AH19" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH19)-ROW($C$5))*32+COLUMN(AH19)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>E470</v>
       </c>
     </row>
@@ -24471,131 +24620,131 @@
         <v>657</v>
       </c>
       <c r="C20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C20)-ROW($C$5))*32+COLUMN(C20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0022</v>
       </c>
       <c r="D20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D20)-ROW($C$5))*32+COLUMN(D20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F7A0</v>
       </c>
       <c r="E20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E20)-ROW($C$5))*32+COLUMN(E20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>EFFE</v>
       </c>
       <c r="F20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F20)-ROW($C$5))*32+COLUMN(F20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0BC0</v>
       </c>
       <c r="G20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G20)-ROW($C$5))*32+COLUMN(G20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>03D2</v>
       </c>
       <c r="H20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H20)-ROW($C$5))*32+COLUMN(H20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F860</v>
       </c>
       <c r="I20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I20)-ROW($C$5))*32+COLUMN(I20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F79E</v>
       </c>
       <c r="J20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J20)-ROW($C$5))*32+COLUMN(J20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0F92</v>
       </c>
       <c r="K20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K20)-ROW($C$5))*32+COLUMN(K20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0390</v>
       </c>
       <c r="L20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L20)-ROW($C$5))*32+COLUMN(L20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FFB0</v>
       </c>
       <c r="M20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M20)-ROW($C$5))*32+COLUMN(M20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F3FE</v>
       </c>
       <c r="N20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N20)-ROW($C$5))*32+COLUMN(N20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0FC0</v>
       </c>
       <c r="O20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O20)-ROW($C$5))*32+COLUMN(O20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0762</v>
       </c>
       <c r="P20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P20)-ROW($C$5))*32+COLUMN(P20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FF70</v>
       </c>
       <c r="Q20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q20)-ROW($C$5))*32+COLUMN(Q20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>EFFE</v>
       </c>
       <c r="R20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R20)-ROW($C$5))*32+COLUMN(R20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1380</v>
       </c>
       <c r="S20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S20)-ROW($C$5))*32+COLUMN(S20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0362</v>
       </c>
       <c r="T20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T20)-ROW($C$5))*32+COLUMN(T20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FFB0</v>
       </c>
       <c r="U20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U20)-ROW($C$5))*32+COLUMN(U20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F42E</v>
       </c>
       <c r="V20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V20)-ROW($C$5))*32+COLUMN(V20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0810</v>
       </c>
       <c r="W20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W20)-ROW($C$5))*32+COLUMN(W20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>07A2</v>
       </c>
       <c r="X20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X20)-ROW($C$5))*32+COLUMN(X20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>07C0</v>
       </c>
       <c r="Y20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y20)-ROW($C$5))*32+COLUMN(Y20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F87E</v>
       </c>
       <c r="Z20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z20)-ROW($C$5))*32+COLUMN(Z20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0C82</v>
       </c>
       <c r="AA20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA20)-ROW($C$5))*32+COLUMN(AA20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0B94</v>
       </c>
       <c r="AB20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB20)-ROW($C$5))*32+COLUMN(AB20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0490</v>
       </c>
       <c r="AC20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC20)-ROW($C$5))*32+COLUMN(AC20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FB90</v>
       </c>
       <c r="AD20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD20)-ROW($C$5))*32+COLUMN(AD20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>1062</v>
       </c>
       <c r="AE20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE20)-ROW($C$5))*32+COLUMN(AE20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0842</v>
       </c>
       <c r="AF20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF20)-ROW($C$5))*32+COLUMN(AF20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>07B0</v>
       </c>
       <c r="AG20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG20)-ROW($C$5))*32+COLUMN(AG20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>EC10</v>
       </c>
       <c r="AH20" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH20)-ROW($C$5))*32+COLUMN(AH20)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0C82</v>
       </c>
     </row>
@@ -24605,131 +24754,131 @@
         <v>658</v>
       </c>
       <c r="C21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C21)-ROW($C$5))*32+COLUMN(C21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0850</v>
       </c>
       <c r="D21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D21)-ROW($C$5))*32+COLUMN(D21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>13E2</v>
       </c>
       <c r="E21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E21)-ROW($C$5))*32+COLUMN(E21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>2360</v>
       </c>
       <c r="F21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F21)-ROW($C$5))*32+COLUMN(F21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0420</v>
       </c>
       <c r="G21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G21)-ROW($C$5))*32+COLUMN(G21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0460</v>
       </c>
       <c r="H21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H21)-ROW($C$5))*32+COLUMN(H21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>10B0</v>
       </c>
       <c r="I21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I21)-ROW($C$5))*32+COLUMN(I21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1FB0</v>
       </c>
       <c r="J21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J21)-ROW($C$5))*32+COLUMN(J21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>03E0</v>
       </c>
       <c r="K21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K21)-ROW($C$5))*32+COLUMN(K21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0B80</v>
       </c>
       <c r="L21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L21)-ROW($C$5))*32+COLUMN(L21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0BF0</v>
       </c>
       <c r="M21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M21)-ROW($C$5))*32+COLUMN(M21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1430</v>
       </c>
       <c r="N21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N21)-ROW($C$5))*32+COLUMN(N21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FC00</v>
       </c>
       <c r="O21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O21)-ROW($C$5))*32+COLUMN(O21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0F90</v>
       </c>
       <c r="P21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P21)-ROW($C$5))*32+COLUMN(P21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0BC2</v>
       </c>
       <c r="Q21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q21)-ROW($C$5))*32+COLUMN(Q21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1BA0</v>
       </c>
       <c r="R21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R21)-ROW($C$5))*32+COLUMN(R21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FFC0</v>
       </c>
       <c r="S21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S21)-ROW($C$5))*32+COLUMN(S21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>07C2</v>
       </c>
       <c r="T21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T21)-ROW($C$5))*32+COLUMN(T21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0B82</v>
       </c>
       <c r="U21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U21)-ROW($C$5))*32+COLUMN(U21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1BF0</v>
       </c>
       <c r="V21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V21)-ROW($C$5))*32+COLUMN(V21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F44E</v>
       </c>
       <c r="W21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W21)-ROW($C$5))*32+COLUMN(W21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0BB2</v>
       </c>
       <c r="X21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X21)-ROW($C$5))*32+COLUMN(X21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0FD2</v>
       </c>
       <c r="Y21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y21)-ROW($C$5))*32+COLUMN(Y21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>14C2</v>
       </c>
       <c r="Z21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z21)-ROW($C$5))*32+COLUMN(Z21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F8A0</v>
       </c>
       <c r="AA21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA21)-ROW($C$5))*32+COLUMN(AA21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0792</v>
       </c>
       <c r="AB21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB21)-ROW($C$5))*32+COLUMN(AB21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0852</v>
       </c>
       <c r="AC21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC21)-ROW($C$5))*32+COLUMN(AC21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>13E2</v>
       </c>
       <c r="AD21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD21)-ROW($C$5))*32+COLUMN(AD21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F850</v>
       </c>
       <c r="AE21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE21)-ROW($C$5))*32+COLUMN(AE21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>00A0</v>
       </c>
       <c r="AF21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF21)-ROW($C$5))*32+COLUMN(AF21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0032</v>
       </c>
       <c r="AG21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG21)-ROW($C$5))*32+COLUMN(AG21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0C22</v>
       </c>
       <c r="AH21" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH21)-ROW($C$5))*32+COLUMN(AH21)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F0D0</v>
       </c>
     </row>
@@ -24739,131 +24888,131 @@
         <v>659</v>
       </c>
       <c r="C22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C22)-ROW($C$5))*32+COLUMN(C22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F452</v>
       </c>
       <c r="D22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D22)-ROW($C$5))*32+COLUMN(D22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>EFE0</v>
       </c>
       <c r="E22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E22)-ROW($C$5))*32+COLUMN(E22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>EF7E</v>
       </c>
       <c r="F22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F22)-ROW($C$5))*32+COLUMN(F22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FC32</v>
       </c>
       <c r="G22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G22)-ROW($C$5))*32+COLUMN(G22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F072</v>
       </c>
       <c r="H22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H22)-ROW($C$5))*32+COLUMN(H22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F4C0</v>
       </c>
       <c r="I22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I22)-ROW($C$5))*32+COLUMN(I22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>EBCE</v>
       </c>
       <c r="J22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J22)-ROW($C$5))*32+COLUMN(J22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>03F0</v>
       </c>
       <c r="K22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K22)-ROW($C$5))*32+COLUMN(K22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FBA2</v>
       </c>
       <c r="L22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L22)-ROW($C$5))*32+COLUMN(L22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F400</v>
       </c>
       <c r="M22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M22)-ROW($C$5))*32+COLUMN(M22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>E45E</v>
       </c>
       <c r="N22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N22)-ROW($C$5))*32+COLUMN(N22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0410</v>
       </c>
       <c r="O22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O22)-ROW($C$5))*32+COLUMN(O22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FFA2</v>
       </c>
       <c r="P22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P22)-ROW($C$5))*32+COLUMN(P22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F7D0</v>
       </c>
       <c r="Q22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q22)-ROW($C$5))*32+COLUMN(Q22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>EBBE</v>
       </c>
       <c r="R22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R22)-ROW($C$5))*32+COLUMN(R22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0BD0</v>
       </c>
       <c r="S22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S22)-ROW($C$5))*32+COLUMN(S22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FBC2</v>
       </c>
       <c r="T22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T22)-ROW($C$5))*32+COLUMN(T22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FB80</v>
       </c>
       <c r="U22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U22)-ROW($C$5))*32+COLUMN(U22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F00E</v>
       </c>
       <c r="V22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V22)-ROW($C$5))*32+COLUMN(V22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0050</v>
       </c>
       <c r="W22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W22)-ROW($C$5))*32+COLUMN(W22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>03D2</v>
       </c>
       <c r="X22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X22)-ROW($C$5))*32+COLUMN(X22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>03D0</v>
       </c>
       <c r="Y22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y22)-ROW($C$5))*32+COLUMN(Y22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F0E0</v>
       </c>
       <c r="Z22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z22)-ROW($C$5))*32+COLUMN(Z22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0CA0</v>
       </c>
       <c r="AA22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA22)-ROW($C$5))*32+COLUMN(AA22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0384</v>
       </c>
       <c r="AB22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB22)-ROW($C$5))*32+COLUMN(AB22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0440</v>
       </c>
       <c r="AC22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC22)-ROW($C$5))*32+COLUMN(AC22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F3EE</v>
       </c>
       <c r="AD22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD22)-ROW($C$5))*32+COLUMN(AD22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0C52</v>
       </c>
       <c r="AE22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE22)-ROW($C$5))*32+COLUMN(AE22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>00A2</v>
       </c>
       <c r="AF22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF22)-ROW($C$5))*32+COLUMN(AF22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0030</v>
       </c>
       <c r="AG22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG22)-ROW($C$5))*32+COLUMN(AG22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>EC20</v>
       </c>
       <c r="AH22" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH22)-ROW($C$5))*32+COLUMN(AH22)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>04C0</v>
       </c>
     </row>
@@ -24873,131 +25022,131 @@
         <v>660</v>
       </c>
       <c r="C23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C23)-ROW($C$5))*32+COLUMN(C23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1022</v>
       </c>
       <c r="D23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D23)-ROW($C$5))*32+COLUMN(D23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0FD2</v>
       </c>
       <c r="E23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E23)-ROW($C$5))*32+COLUMN(E23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>1F80</v>
       </c>
       <c r="F23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F23)-ROW($C$5))*32+COLUMN(F23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>03F0</v>
       </c>
       <c r="G23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G23)-ROW($C$5))*32+COLUMN(G23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0830</v>
       </c>
       <c r="H23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H23)-ROW($C$5))*32+COLUMN(H23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0C82</v>
       </c>
       <c r="I23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I23)-ROW($C$5))*32+COLUMN(I23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>17E0</v>
       </c>
       <c r="J23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J23)-ROW($C$5))*32+COLUMN(J23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FFB0</v>
       </c>
       <c r="K23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K23)-ROW($C$5))*32+COLUMN(K23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0410</v>
       </c>
       <c r="L23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L23)-ROW($C$5))*32+COLUMN(L23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0432</v>
       </c>
       <c r="M23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M23)-ROW($C$5))*32+COLUMN(M23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0870</v>
       </c>
       <c r="N23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N23)-ROW($C$5))*32+COLUMN(N23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F48E</v>
       </c>
       <c r="O23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O23)-ROW($C$5))*32+COLUMN(O23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0BD0</v>
       </c>
       <c r="P23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P23)-ROW($C$5))*32+COLUMN(P23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>07B2</v>
       </c>
       <c r="Q23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q23)-ROW($C$5))*32+COLUMN(Q23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0F90</v>
       </c>
       <c r="R23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R23)-ROW($C$5))*32+COLUMN(R23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FBB0</v>
       </c>
       <c r="S23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S23)-ROW($C$5))*32+COLUMN(S23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FFF0</v>
       </c>
       <c r="T23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T23)-ROW($C$5))*32+COLUMN(T23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>07A2</v>
       </c>
       <c r="U23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U23)-ROW($C$5))*32+COLUMN(U23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1410</v>
       </c>
       <c r="V23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V23)-ROW($C$5))*32+COLUMN(V23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F410</v>
       </c>
       <c r="W23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W23)-ROW($C$5))*32+COLUMN(W23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0022</v>
       </c>
       <c r="X23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X23)-ROW($C$5))*32+COLUMN(X23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0BC2</v>
       </c>
       <c r="Y23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y23)-ROW($C$5))*32+COLUMN(Y23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0CE0</v>
       </c>
       <c r="Z23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z23)-ROW($C$5))*32+COLUMN(Z23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F850</v>
       </c>
       <c r="AA23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA23)-ROW($C$5))*32+COLUMN(AA23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FFB2</v>
       </c>
       <c r="AB23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB23)-ROW($C$5))*32+COLUMN(AB23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0490</v>
       </c>
       <c r="AC23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC23)-ROW($C$5))*32+COLUMN(AC23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0BC0</v>
       </c>
       <c r="AD23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD23)-ROW($C$5))*32+COLUMN(AD23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>ECC0</v>
       </c>
       <c r="AE23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE23)-ROW($C$5))*32+COLUMN(AE23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FC70</v>
       </c>
       <c r="AF23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF23)-ROW($C$5))*32+COLUMN(AF23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0012</v>
       </c>
       <c r="AG23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG23)-ROW($C$5))*32+COLUMN(AG23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0400</v>
       </c>
       <c r="AH23" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH23)-ROW($C$5))*32+COLUMN(AH23)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F0B2</v>
       </c>
     </row>
@@ -25007,131 +25156,131 @@
         <v>661</v>
       </c>
       <c r="C24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C24)-ROW($C$5))*32+COLUMN(C24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0402</v>
       </c>
       <c r="D24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D24)-ROW($C$5))*32+COLUMN(D24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F7D0</v>
       </c>
       <c r="E24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E24)-ROW($C$5))*32+COLUMN(E24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F37E</v>
       </c>
       <c r="F24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F24)-ROW($C$5))*32+COLUMN(F24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0BF2</v>
       </c>
       <c r="G24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G24)-ROW($C$5))*32+COLUMN(G24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0022</v>
       </c>
       <c r="H24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H24)-ROW($C$5))*32+COLUMN(H24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FC90</v>
       </c>
       <c r="I24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I24)-ROW($C$5))*32+COLUMN(I24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>EFFE</v>
       </c>
       <c r="J24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J24)-ROW($C$5))*32+COLUMN(J24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>0FC2</v>
       </c>
       <c r="K24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K24)-ROW($C$5))*32+COLUMN(K24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>FC12</v>
       </c>
       <c r="L24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L24)-ROW($C$5))*32+COLUMN(L24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="3"/>
         <v>F84E</v>
       </c>
       <c r="M24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M24)-ROW($C$5))*32+COLUMN(M24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>E87E</v>
       </c>
       <c r="N24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N24)-ROW($C$5))*32+COLUMN(N24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0480</v>
       </c>
       <c r="O24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O24)-ROW($C$5))*32+COLUMN(O24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>07E2</v>
       </c>
       <c r="P24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P24)-ROW($C$5))*32+COLUMN(P24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>FFB0</v>
       </c>
       <c r="Q24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q24)-ROW($C$5))*32+COLUMN(Q24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F7AE</v>
       </c>
       <c r="R24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R24)-ROW($C$5))*32+COLUMN(R24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0FC0</v>
       </c>
       <c r="S24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S24)-ROW($C$5))*32+COLUMN(S24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>0002</v>
       </c>
       <c r="T24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T24)-ROW($C$5))*32+COLUMN(T24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>07A0</v>
       </c>
       <c r="U24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U24)-ROW($C$5))*32+COLUMN(U24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>F81E</v>
       </c>
       <c r="V24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V24)-ROW($C$5))*32+COLUMN(V24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="4"/>
         <v>1002</v>
       </c>
       <c r="W24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W24)-ROW($C$5))*32+COLUMN(W24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0422</v>
       </c>
       <c r="X24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X24)-ROW($C$5))*32+COLUMN(X24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0FD0</v>
       </c>
       <c r="Y24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y24)-ROW($C$5))*32+COLUMN(Y24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>F8CE</v>
       </c>
       <c r="Z24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z24)-ROW($C$5))*32+COLUMN(Z24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>1842</v>
       </c>
       <c r="AA24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA24)-ROW($C$5))*32+COLUMN(AA24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>07A4</v>
       </c>
       <c r="AB24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB24)-ROW($C$5))*32+COLUMN(AB24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0880</v>
       </c>
       <c r="AC24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC24)-ROW($C$5))*32+COLUMN(AC24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FBB0</v>
       </c>
       <c r="AD24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD24)-ROW($C$5))*32+COLUMN(AD24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0CB0</v>
       </c>
       <c r="AE24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE24)-ROW($C$5))*32+COLUMN(AE24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0C62</v>
       </c>
       <c r="AF24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF24)-ROW($C$5))*32+COLUMN(AF24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>0BF0</v>
       </c>
       <c r="AG24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG24)-ROW($C$5))*32+COLUMN(AG24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>FBF0</v>
       </c>
       <c r="AH24" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH24)-ROW($C$5))*32+COLUMN(AH24)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="5"/>
         <v>10A0</v>
       </c>
     </row>
@@ -25141,131 +25290,131 @@
         <v>662</v>
       </c>
       <c r="C25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C25)-ROW($C$5))*32+COLUMN(C25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ref="C25:L30" ca="1" si="6">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C25)-ROW($C$5))*32+COLUMN(C25)-COLUMN($C$5),,,"Input data"))</f>
         <v>F030</v>
       </c>
       <c r="D25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D25)-ROW($C$5))*32+COLUMN(D25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>07D2</v>
       </c>
       <c r="E25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E25)-ROW($C$5))*32+COLUMN(E25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0BE0</v>
       </c>
       <c r="F25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F25)-ROW($C$5))*32+COLUMN(F25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F800</v>
       </c>
       <c r="G25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G25)-ROW($C$5))*32+COLUMN(G25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>ECA0</v>
       </c>
       <c r="H25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H25)-ROW($C$5))*32+COLUMN(H25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0482</v>
       </c>
       <c r="I25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I25)-ROW($C$5))*32+COLUMN(I25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0830</v>
       </c>
       <c r="J25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J25)-ROW($C$5))*32+COLUMN(J25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>FBE0</v>
       </c>
       <c r="K25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K25)-ROW($C$5))*32+COLUMN(K25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F040</v>
       </c>
       <c r="L25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L25)-ROW($C$5))*32+COLUMN(L25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>FC80</v>
       </c>
       <c r="M25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M25)-ROW($C$5))*32+COLUMN(M25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ref="M25:V30" ca="1" si="7">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M25)-ROW($C$5))*32+COLUMN(M25)-COLUMN($C$5),,,"Input data"))</f>
         <v>0810</v>
       </c>
       <c r="N25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N25)-ROW($C$5))*32+COLUMN(N25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F030</v>
       </c>
       <c r="O25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O25)-ROW($C$5))*32+COLUMN(O25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F410</v>
       </c>
       <c r="P25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P25)-ROW($C$5))*32+COLUMN(P25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F830</v>
       </c>
       <c r="Q25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q25)-ROW($C$5))*32+COLUMN(Q25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0BA0</v>
       </c>
       <c r="R25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R25)-ROW($C$5))*32+COLUMN(R25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F7A0</v>
       </c>
       <c r="S25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S25)-ROW($C$5))*32+COLUMN(S25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F3D2</v>
       </c>
       <c r="T25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T25)-ROW($C$5))*32+COLUMN(T25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>FFF2</v>
       </c>
       <c r="U25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U25)-ROW($C$5))*32+COLUMN(U25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0840</v>
       </c>
       <c r="V25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V25)-ROW($C$5))*32+COLUMN(V25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>EFF0</v>
       </c>
       <c r="W25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W25)-ROW($C$5))*32+COLUMN(W25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ref="W25:AH30" ca="1" si="8">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W25)-ROW($C$5))*32+COLUMN(W25)-COLUMN($C$5),,,"Input data"))</f>
         <v>F400</v>
       </c>
       <c r="X25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X25)-ROW($C$5))*32+COLUMN(X25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>03B2</v>
       </c>
       <c r="Y25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y25)-ROW($C$5))*32+COLUMN(Y25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0872</v>
       </c>
       <c r="Z25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z25)-ROW($C$5))*32+COLUMN(Z25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>F030</v>
       </c>
       <c r="AA25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA25)-ROW($C$5))*32+COLUMN(AA25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>EFB2</v>
       </c>
       <c r="AB25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB25)-ROW($C$5))*32+COLUMN(AB25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0042</v>
       </c>
       <c r="AC25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC25)-ROW($C$5))*32+COLUMN(AC25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>03B2</v>
       </c>
       <c r="AD25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD25)-ROW($C$5))*32+COLUMN(AD25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>EC40</v>
       </c>
       <c r="AE25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE25)-ROW($C$5))*32+COLUMN(AE25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FFE0</v>
       </c>
       <c r="AF25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF25)-ROW($C$5))*32+COLUMN(AF25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FFE2</v>
       </c>
       <c r="AG25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG25)-ROW($C$5))*32+COLUMN(AG25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0012</v>
       </c>
       <c r="AH25" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH25)-ROW($C$5))*32+COLUMN(AH25)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>F420</v>
       </c>
     </row>
@@ -25275,131 +25424,131 @@
         <v>663</v>
       </c>
       <c r="C26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C26)-ROW($C$5))*32+COLUMN(C26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F422</v>
       </c>
       <c r="D26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D26)-ROW($C$5))*32+COLUMN(D26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F7B0</v>
       </c>
       <c r="E26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E26)-ROW($C$5))*32+COLUMN(E26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>E7CE</v>
       </c>
       <c r="F26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F26)-ROW($C$5))*32+COLUMN(F26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0BD2</v>
       </c>
       <c r="G26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G26)-ROW($C$5))*32+COLUMN(G26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F080</v>
       </c>
       <c r="H26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H26)-ROW($C$5))*32+COLUMN(H26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0070</v>
       </c>
       <c r="I26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I26)-ROW($C$5))*32+COLUMN(I26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>EC2E</v>
       </c>
       <c r="J26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J26)-ROW($C$5))*32+COLUMN(J26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0FE2</v>
       </c>
       <c r="K26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K26)-ROW($C$5))*32+COLUMN(K26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F850</v>
       </c>
       <c r="L26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L26)-ROW($C$5))*32+COLUMN(L26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0070</v>
       </c>
       <c r="M26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M26)-ROW($C$5))*32+COLUMN(M26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F00E</v>
       </c>
       <c r="N26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N26)-ROW($C$5))*32+COLUMN(N26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0C42</v>
       </c>
       <c r="O26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O26)-ROW($C$5))*32+COLUMN(O26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0020</v>
       </c>
       <c r="P26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P26)-ROW($C$5))*32+COLUMN(P26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0030</v>
       </c>
       <c r="Q26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q26)-ROW($C$5))*32+COLUMN(Q26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F7AE</v>
       </c>
       <c r="R26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R26)-ROW($C$5))*32+COLUMN(R26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>17B2</v>
       </c>
       <c r="S26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S26)-ROW($C$5))*32+COLUMN(S26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>03D2</v>
       </c>
       <c r="T26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T26)-ROW($C$5))*32+COLUMN(T26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0400</v>
       </c>
       <c r="U26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U26)-ROW($C$5))*32+COLUMN(U26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F84E</v>
       </c>
       <c r="V26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V26)-ROW($C$5))*32+COLUMN(V26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>17F0</v>
       </c>
       <c r="W26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W26)-ROW($C$5))*32+COLUMN(W26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0BE2</v>
       </c>
       <c r="X26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X26)-ROW($C$5))*32+COLUMN(X26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>13A0</v>
       </c>
       <c r="Y26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y26)-ROW($C$5))*32+COLUMN(Y26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FC4E</v>
       </c>
       <c r="Z26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z26)-ROW($C$5))*32+COLUMN(Z26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1820</v>
       </c>
       <c r="AA26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA26)-ROW($C$5))*32+COLUMN(AA26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0792</v>
       </c>
       <c r="AB26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB26)-ROW($C$5))*32+COLUMN(AB26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1020</v>
       </c>
       <c r="AC26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC26)-ROW($C$5))*32+COLUMN(AC26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FB9E</v>
       </c>
       <c r="AD26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD26)-ROW($C$5))*32+COLUMN(AD26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1C10</v>
       </c>
       <c r="AE26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE26)-ROW($C$5))*32+COLUMN(AE26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1BC2</v>
       </c>
       <c r="AF26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF26)-ROW($C$5))*32+COLUMN(AF26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>13C0</v>
       </c>
       <c r="AG26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG26)-ROW($C$5))*32+COLUMN(AG26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FBE0</v>
       </c>
       <c r="AH26" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH26)-ROW($C$5))*32+COLUMN(AH26)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>2002</v>
       </c>
     </row>
@@ -25409,131 +25558,131 @@
         <v>664</v>
       </c>
       <c r="C27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C27)-ROW($C$5))*32+COLUMN(C27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F040</v>
       </c>
       <c r="D27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D27)-ROW($C$5))*32+COLUMN(D27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>13A2</v>
       </c>
       <c r="E27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E27)-ROW($C$5))*32+COLUMN(E27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0F80</v>
       </c>
       <c r="F27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F27)-ROW($C$5))*32+COLUMN(F27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>FC30</v>
       </c>
       <c r="G27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G27)-ROW($C$5))*32+COLUMN(G27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F46E</v>
       </c>
       <c r="H27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H27)-ROW($C$5))*32+COLUMN(H27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0CC2</v>
       </c>
       <c r="I27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I27)-ROW($C$5))*32+COLUMN(I27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>17B2</v>
       </c>
       <c r="J27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J27)-ROW($C$5))*32+COLUMN(J27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0010</v>
       </c>
       <c r="K27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K27)-ROW($C$5))*32+COLUMN(K27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>FC10</v>
       </c>
       <c r="L27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L27)-ROW($C$5))*32+COLUMN(L27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0872</v>
       </c>
       <c r="M27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M27)-ROW($C$5))*32+COLUMN(M27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>1000</v>
       </c>
       <c r="N27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N27)-ROW($C$5))*32+COLUMN(N27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F8B0</v>
       </c>
       <c r="O27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O27)-ROW($C$5))*32+COLUMN(O27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>07BE</v>
       </c>
       <c r="P27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P27)-ROW($C$5))*32+COLUMN(P27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0BE2</v>
       </c>
       <c r="Q27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q27)-ROW($C$5))*32+COLUMN(Q27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>13B0</v>
       </c>
       <c r="R27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R27)-ROW($C$5))*32+COLUMN(R27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>FFE0</v>
       </c>
       <c r="S27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S27)-ROW($C$5))*32+COLUMN(S27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F410</v>
       </c>
       <c r="T27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T27)-ROW($C$5))*32+COLUMN(T27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0450</v>
       </c>
       <c r="U27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U27)-ROW($C$5))*32+COLUMN(U27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0C70</v>
       </c>
       <c r="V27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V27)-ROW($C$5))*32+COLUMN(V27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F420</v>
       </c>
       <c r="W27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W27)-ROW($C$5))*32+COLUMN(W27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>03C0</v>
       </c>
       <c r="X27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X27)-ROW($C$5))*32+COLUMN(X27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0F82</v>
       </c>
       <c r="Y27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y27)-ROW($C$5))*32+COLUMN(Y27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1060</v>
       </c>
       <c r="Z27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z27)-ROW($C$5))*32+COLUMN(Z27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FFE0</v>
       </c>
       <c r="AA27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA27)-ROW($C$5))*32+COLUMN(AA27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FB70</v>
       </c>
       <c r="AB27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB27)-ROW($C$5))*32+COLUMN(AB27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>13D2</v>
       </c>
       <c r="AC27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC27)-ROW($C$5))*32+COLUMN(AC27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0F90</v>
       </c>
       <c r="AD27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD27)-ROW($C$5))*32+COLUMN(AD27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>F820</v>
       </c>
       <c r="AE27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE27)-ROW($C$5))*32+COLUMN(AE27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FC40</v>
       </c>
       <c r="AF27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF27)-ROW($C$5))*32+COLUMN(AF27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0FA2</v>
       </c>
       <c r="AG27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG27)-ROW($C$5))*32+COLUMN(AG27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0BE2</v>
       </c>
       <c r="AH27" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH27)-ROW($C$5))*32+COLUMN(AH27)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FC60</v>
       </c>
     </row>
@@ -25543,131 +25692,131 @@
         <v>665</v>
       </c>
       <c r="C28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C28)-ROW($C$5))*32+COLUMN(C28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F012</v>
       </c>
       <c r="D28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D28)-ROW($C$5))*32+COLUMN(D28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>FB80</v>
       </c>
       <c r="E28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E28)-ROW($C$5))*32+COLUMN(E28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>EB5E</v>
       </c>
       <c r="F28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F28)-ROW($C$5))*32+COLUMN(F28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0802</v>
       </c>
       <c r="G28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G28)-ROW($C$5))*32+COLUMN(G28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F420</v>
       </c>
       <c r="H28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H28)-ROW($C$5))*32+COLUMN(H28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0090</v>
       </c>
       <c r="I28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I28)-ROW($C$5))*32+COLUMN(I28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F78E</v>
       </c>
       <c r="J28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J28)-ROW($C$5))*32+COLUMN(J28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>13E2</v>
       </c>
       <c r="K28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K28)-ROW($C$5))*32+COLUMN(K28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>FC02</v>
       </c>
       <c r="L28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L28)-ROW($C$5))*32+COLUMN(L28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0060</v>
       </c>
       <c r="M28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M28)-ROW($C$5))*32+COLUMN(M28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F40E</v>
       </c>
       <c r="N28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N28)-ROW($C$5))*32+COLUMN(N28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>1090</v>
       </c>
       <c r="O28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O28)-ROW($C$5))*32+COLUMN(O28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0F90</v>
       </c>
       <c r="P28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P28)-ROW($C$5))*32+COLUMN(P28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0BD0</v>
       </c>
       <c r="Q28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q28)-ROW($C$5))*32+COLUMN(Q28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>FBAE</v>
       </c>
       <c r="R28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R28)-ROW($C$5))*32+COLUMN(R28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>1FD2</v>
       </c>
       <c r="S28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S28)-ROW($C$5))*32+COLUMN(S28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0002</v>
       </c>
       <c r="T28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T28)-ROW($C$5))*32+COLUMN(T28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0820</v>
       </c>
       <c r="U28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U28)-ROW($C$5))*32+COLUMN(U28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F85E</v>
       </c>
       <c r="V28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V28)-ROW($C$5))*32+COLUMN(V28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>1800</v>
       </c>
       <c r="W28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W28)-ROW($C$5))*32+COLUMN(W28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0F82</v>
       </c>
       <c r="X28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X28)-ROW($C$5))*32+COLUMN(X28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1B60</v>
       </c>
       <c r="Y28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y28)-ROW($C$5))*32+COLUMN(Y28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FC3E</v>
       </c>
       <c r="Z28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z28)-ROW($C$5))*32+COLUMN(Z28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>23C2</v>
       </c>
       <c r="AA28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA28)-ROW($C$5))*32+COLUMN(AA28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0B42</v>
       </c>
       <c r="AB28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB28)-ROW($C$5))*32+COLUMN(AB28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1BA0</v>
       </c>
       <c r="AC28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC28)-ROW($C$5))*32+COLUMN(AC28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FF7E</v>
       </c>
       <c r="AD28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD28)-ROW($C$5))*32+COLUMN(AD28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>27E0</v>
       </c>
       <c r="AE28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE28)-ROW($C$5))*32+COLUMN(AE28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1012</v>
       </c>
       <c r="AF28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF28)-ROW($C$5))*32+COLUMN(AF28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1B70</v>
       </c>
       <c r="AG28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG28)-ROW($C$5))*32+COLUMN(AG28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FFC0</v>
       </c>
       <c r="AH28" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH28)-ROW($C$5))*32+COLUMN(AH28)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>2040</v>
       </c>
     </row>
@@ -25677,131 +25826,131 @@
         <v>666</v>
       </c>
       <c r="C29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C29)-ROW($C$5))*32+COLUMN(C29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>FC70</v>
       </c>
       <c r="D29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D29)-ROW($C$5))*32+COLUMN(D29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>1BA2</v>
       </c>
       <c r="E29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E29)-ROW($C$5))*32+COLUMN(E29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0FA0</v>
       </c>
       <c r="F29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F29)-ROW($C$5))*32+COLUMN(F29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0BA0</v>
       </c>
       <c r="G29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G29)-ROW($C$5))*32+COLUMN(G29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0002</v>
       </c>
       <c r="H29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H29)-ROW($C$5))*32+COLUMN(H29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>1432</v>
       </c>
       <c r="I29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I29)-ROW($C$5))*32+COLUMN(I29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0FE0</v>
       </c>
       <c r="J29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J29)-ROW($C$5))*32+COLUMN(J29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0010</v>
       </c>
       <c r="K29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K29)-ROW($C$5))*32+COLUMN(K29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F83E</v>
       </c>
       <c r="L29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L29)-ROW($C$5))*32+COLUMN(L29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>13E0</v>
       </c>
       <c r="M29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M29)-ROW($C$5))*32+COLUMN(M29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>085E</v>
       </c>
       <c r="N29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N29)-ROW($C$5))*32+COLUMN(N29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>07E0</v>
       </c>
       <c r="O29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O29)-ROW($C$5))*32+COLUMN(O29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>005E</v>
       </c>
       <c r="P29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P29)-ROW($C$5))*32+COLUMN(P29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0842</v>
       </c>
       <c r="Q29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q29)-ROW($C$5))*32+COLUMN(Q29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0FEE</v>
       </c>
       <c r="R29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R29)-ROW($C$5))*32+COLUMN(R29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>03D0</v>
       </c>
       <c r="S29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S29)-ROW($C$5))*32+COLUMN(S29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>FC20</v>
       </c>
       <c r="T29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T29)-ROW($C$5))*32+COLUMN(T29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0FE2</v>
       </c>
       <c r="U29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U29)-ROW($C$5))*32+COLUMN(U29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>1400</v>
       </c>
       <c r="V29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V29)-ROW($C$5))*32+COLUMN(V29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0780</v>
       </c>
       <c r="W29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W29)-ROW($C$5))*32+COLUMN(W29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0B90</v>
       </c>
       <c r="X29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X29)-ROW($C$5))*32+COLUMN(X29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1772</v>
       </c>
       <c r="Y29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y29)-ROW($C$5))*32+COLUMN(Y29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1410</v>
       </c>
       <c r="Z29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z29)-ROW($C$5))*32+COLUMN(Z29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>07B0</v>
       </c>
       <c r="AA29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA29)-ROW($C$5))*32+COLUMN(AA29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FB10</v>
       </c>
       <c r="AB29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB29)-ROW($C$5))*32+COLUMN(AB29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>17F2</v>
       </c>
       <c r="AC29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC29)-ROW($C$5))*32+COLUMN(AC29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0B20</v>
       </c>
       <c r="AD29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD29)-ROW($C$5))*32+COLUMN(AD29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>03F0</v>
       </c>
       <c r="AE29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE29)-ROW($C$5))*32+COLUMN(AE29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>FC1E</v>
       </c>
       <c r="AF29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF29)-ROW($C$5))*32+COLUMN(AF29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>17B2</v>
       </c>
       <c r="AG29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG29)-ROW($C$5))*32+COLUMN(AG29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>07CE</v>
       </c>
       <c r="AH29" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH29)-ROW($C$5))*32+COLUMN(AH29)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0830</v>
       </c>
     </row>
@@ -25811,131 +25960,131 @@
         <v>667</v>
       </c>
       <c r="C30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(C30)-ROW($C$5))*32+COLUMN(C30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>E050</v>
       </c>
       <c r="D30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(D30)-ROW($C$5))*32+COLUMN(D30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>EF80</v>
       </c>
       <c r="E30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(E30)-ROW($C$5))*32+COLUMN(E30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>D38E</v>
       </c>
       <c r="F30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(F30)-ROW($C$5))*32+COLUMN(F30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>0382</v>
       </c>
       <c r="G30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(G30)-ROW($C$5))*32+COLUMN(G30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>EBE0</v>
       </c>
       <c r="H30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(H30)-ROW($C$5))*32+COLUMN(H30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>F810</v>
       </c>
       <c r="I30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(I30)-ROW($C$5))*32+COLUMN(I30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>DFBE</v>
       </c>
       <c r="J30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(J30)-ROW($C$5))*32+COLUMN(J30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>07D0</v>
       </c>
       <c r="K30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(K30)-ROW($C$5))*32+COLUMN(K30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>EC10</v>
       </c>
       <c r="L30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(L30)-ROW($C$5))*32+COLUMN(L30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="6"/>
         <v>FFC0</v>
       </c>
       <c r="M30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(M30)-ROW($C$5))*32+COLUMN(M30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>E01E</v>
       </c>
       <c r="N30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(N30)-ROW($C$5))*32+COLUMN(N30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0BB0</v>
       </c>
       <c r="O30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(O30)-ROW($C$5))*32+COLUMN(O30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F820</v>
       </c>
       <c r="P30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(P30)-ROW($C$5))*32+COLUMN(P30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F810</v>
       </c>
       <c r="Q30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Q30)-ROW($C$5))*32+COLUMN(Q30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>EBBE</v>
       </c>
       <c r="R30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(R30)-ROW($C$5))*32+COLUMN(R30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>0BA0</v>
       </c>
       <c r="S30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(S30)-ROW($C$5))*32+COLUMN(S30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>FBF0</v>
       </c>
       <c r="T30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(T30)-ROW($C$5))*32+COLUMN(T30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>07A0</v>
       </c>
       <c r="U30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(U30)-ROW($C$5))*32+COLUMN(U30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>F3EE</v>
       </c>
       <c r="V30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(V30)-ROW($C$5))*32+COLUMN(V30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="7"/>
         <v>1B50</v>
       </c>
       <c r="W30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(W30)-ROW($C$5))*32+COLUMN(W30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0752</v>
       </c>
       <c r="X30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(X30)-ROW($C$5))*32+COLUMN(X30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0F30</v>
       </c>
       <c r="Y30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Y30)-ROW($C$5))*32+COLUMN(Y30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>F7EE</v>
       </c>
       <c r="Z30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(Z30)-ROW($C$5))*32+COLUMN(Z30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1B80</v>
       </c>
       <c r="AA30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AA30)-ROW($C$5))*32+COLUMN(AA30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>02F2</v>
       </c>
       <c r="AB30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AB30)-ROW($C$5))*32+COLUMN(AB30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0FD0</v>
       </c>
       <c r="AC30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AC30)-ROW($C$5))*32+COLUMN(AC30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>F70E</v>
       </c>
       <c r="AD30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AD30)-ROW($C$5))*32+COLUMN(AD30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>13C0</v>
       </c>
       <c r="AE30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AE30)-ROW($C$5))*32+COLUMN(AE30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>0BE0</v>
       </c>
       <c r="AF30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AF30)-ROW($C$5))*32+COLUMN(AF30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1390</v>
       </c>
       <c r="AG30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AG30)-ROW($C$5))*32+COLUMN(AG30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>F79E</v>
       </c>
       <c r="AH30" s="4" t="str">
-        <f ca="1">INDIRECT(ADDRESS(ROW($B$4),COLUMN($B$4)+(ROW(AH30)-ROW($C$5))*32+COLUMN(AH30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ca="1" si="8"/>
         <v>1C00</v>
       </c>
       <c r="AI30" s="3"/>
@@ -51242,8 +51391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AH114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52467,7 +52616,7 @@
         <v>FFA8</v>
       </c>
       <c r="K13" s="17" t="str">
-        <f t="shared" ref="K13:Z29" ca="1" si="2">INDIRECT(ADDRESS(ROW($B$4)+4,COLUMN($B$4)+(ROW(K13)-ROW($C$5))*32+COLUMN(K13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ref="K13:Z28" ca="1" si="2">INDIRECT(ADDRESS(ROW($B$4)+4,COLUMN($B$4)+(ROW(K13)-ROW($C$5))*32+COLUMN(K13)-COLUMN($C$5),,,"Input data"))</f>
         <v>FFBB</v>
       </c>
       <c r="L13" s="17" t="str">
@@ -52531,7 +52680,7 @@
         <v>FFA2</v>
       </c>
       <c r="AA13" s="17" t="str">
-        <f t="shared" ref="AA13:AH29" ca="1" si="3">INDIRECT(ADDRESS(ROW($B$4)+4,COLUMN($B$4)+(ROW(AA13)-ROW($C$5))*32+COLUMN(AA13)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ref="AA13:AH28" ca="1" si="3">INDIRECT(ADDRESS(ROW($B$4)+4,COLUMN($B$4)+(ROW(AA13)-ROW($C$5))*32+COLUMN(AA13)-COLUMN($C$5),,,"Input data"))</f>
         <v>FFB4</v>
       </c>
       <c r="AB13" s="17" t="str">
@@ -54696,7 +54845,7 @@
         <v>4115</v>
       </c>
       <c r="C30" s="17" t="str">
-        <f t="shared" ref="C30:R31" ca="1" si="5">INDIRECT(ADDRESS(ROW($B$4)+4,COLUMN($B$4)+(ROW(C30)-ROW($C$5))*32+COLUMN(C30)-COLUMN($C$5),,,"Input data"))</f>
+        <f t="shared" ref="C30:I31" ca="1" si="5">INDIRECT(ADDRESS(ROW($B$4)+4,COLUMN($B$4)+(ROW(C30)-ROW($C$5))*32+COLUMN(C30)-COLUMN($C$5),,,"Input data"))</f>
         <v>0695</v>
       </c>
       <c r="D30" s="17" t="str">

</xml_diff>